<commit_message>
Validacao customizada: email nao repetido na atualizacao de Cliente
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="164">
   <si>
     <t>nome aula</t>
   </si>
@@ -690,6 +690,15 @@
   </si>
   <si>
     <t>0:50 - Anotação @Column(unique=true) ... aprendido sobre o atributo "unique", que garante que o campo da entidade nao receba dados repetidos.. uma forma de dizer também que o campo pode ser numa chave candidata</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Validação customizada: email não repetido na atualização de Cliente</t>
+  </si>
+  <si>
+    <t>5:13 - estrutura Map&lt;String,String&gt; - responsável por captar parametros recebidos pela URI</t>
+  </si>
+  <si>
+    <t>4:50 - HttpServletRequest - tem função que permite obter parametros passados pela URI</t>
   </si>
 </sst>
 </file>
@@ -911,8 +920,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G99" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G99"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G101" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G101"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1180,7 +1189,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1188,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G99"/>
+  <dimension ref="B1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2968,7 +2977,7 @@
     </row>
     <row r="96" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B96" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>125</v>
@@ -2988,7 +2997,7 @@
     </row>
     <row r="97" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B97" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>125</v>
@@ -3006,7 +3015,7 @@
     </row>
     <row r="98" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B98" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>125</v>
@@ -3024,7 +3033,7 @@
     </row>
     <row r="99" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B99" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>125</v>
@@ -3039,6 +3048,44 @@
         <v>157</v>
       </c>
       <c r="G99" s="10"/>
+    </row>
+    <row r="100" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B100" s="8">
+        <v>3</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D100" s="8">
+        <v>47</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G100" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B101" s="8">
+        <v>3</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D101" s="8">
+        <v>47</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="G101" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Aulas: Apresentando caso de uso e Nivelamento sobre SQL e JPQL - commit somente da planilha de anotecoes atualizada - sem modificacoes no projeto
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="169">
   <si>
     <t>nome aula</t>
   </si>
@@ -699,6 +699,23 @@
   </si>
   <si>
     <t>4:50 - HttpServletRequest - tem função que permite obter parametros passados pela URI</t>
+  </si>
+  <si>
+    <t>0:44 - discussão sobre Caso de Uso - descreve o cenário de utilização da aplicação...</t>
+  </si>
+  <si>
+    <t>1:27 - exemplo/comparativo entre uma consulta feita com SQL e uma consulta feita com JPQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+9:31 - sintaxe INNER JOIN em SQl e JPQL</t>
+  </si>
+  <si>
+    <t>0:34 - JPQL é a linguagem de consulta da JPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+12:48 - instrução SELECT DISTINCT - faz uma consulta no banco de dados e retorna objetos sem repetição</t>
   </si>
 </sst>
 </file>
@@ -920,8 +937,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G101" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G101"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G106" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G106"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1189,7 +1206,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1197,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G101"/>
+  <dimension ref="B1:G106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,7 +1225,7 @@
     <col min="1" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="42.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="79.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="120" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
@@ -3087,6 +3104,88 @@
       </c>
       <c r="G101" s="10"/>
     </row>
+    <row r="102" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B102" s="8">
+        <v>3</v>
+      </c>
+      <c r="C102" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D102" s="8">
+        <v>48</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="F102" s="9"/>
+      <c r="G102" s="10"/>
+    </row>
+    <row r="103" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B103" s="8">
+        <v>3</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D103" s="8">
+        <v>49</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G103" s="10"/>
+    </row>
+    <row r="104" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B104" s="8">
+        <v>3</v>
+      </c>
+      <c r="C104" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D104" s="8">
+        <v>49</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F104" s="9"/>
+      <c r="G104" s="10"/>
+    </row>
+    <row r="105" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B105" s="8">
+        <v>3</v>
+      </c>
+      <c r="C105" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D105" s="8">
+        <v>49</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F105" s="9"/>
+      <c r="G105" s="10"/>
+    </row>
+    <row r="106" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B106" s="8">
+        <v>3</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D106" s="8">
+        <v>49</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="F106" s="9"/>
+      <c r="G106" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Busca de produtos por nome e categorias
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="8205"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="185">
   <si>
     <t>nome aula</t>
   </si>
@@ -717,11 +718,81 @@
     <t xml:space="preserve">
 12:48 - instrução SELECT DISTINCT - faz uma consulta no banco de dados e retorna objetos sem repetição</t>
   </si>
+  <si>
+    <t>Apresentando o caso de uso</t>
+  </si>
+  <si>
+    <t>Nivelamento sobre SQL e JPQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Busca de pedidos por nome e categorias - PARTE 1</t>
+  </si>
+  <si>
+    <t>5:22 - criação do metodo search com paginação da classe ProdutoService</t>
+  </si>
+  <si>
+    <t>4:20 - criação de um novo service, no caso ProdutoService</t>
+  </si>
+  <si>
+    <t>9:26 - Spring Data - na documentação mostra os "Query Methods"... são metodos que utilizam da nomeação padrao de nomes de metodos para gerar automaticamente a lógica de consulta ... util pois nao precisa implementar alguns metodos</t>
+  </si>
+  <si>
+    <t>10:41 - anotação @Param - responsável por pegar o valor do parâmetro passado no método (search) com a anotação @Query e passar para o parâmetro da consulta JPQL... neste caso, nomeamos o parâmetro da JPQL como "%:nome%"</t>
+  </si>
+  <si>
+    <t>10:30 - anotação @Query("INSIRA SUA JPQL") do framework Spring Data- utilizada na interface de repositórios. o framework faz um pré-processamento e cria automaticamente o metodo sem precisar a criar uma nova classe</t>
+  </si>
+  <si>
+    <t>14:11 - criação da classe ProdutoDTO</t>
+  </si>
+  <si>
+    <t>15:20 - o metodo GET não aceita enviar parametros no corpo da requisição .. como o POST ... somente aceita como parametros na URL</t>
+  </si>
+  <si>
+    <t>18:11 - criação de classe auxiliar URL</t>
+  </si>
+  <si>
+    <t>12:42 - criação do end point ProdutoResource</t>
+  </si>
+  <si>
+    <t>Busca de pedidos por nome e categorias - PARTE 2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5:37 - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>F A N T Á S T I C O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> - dica de uso do padrao de nomes do framework descrito na documentação, para que o próprio framework se encarregue de gerar as consultas JPQL invés de criarmos as consultas/sintaxes na unha</t>
+    </r>
+  </si>
+  <si>
+    <t>1:52 - criação de metodo de encode - que formata a URL eliminando caracteres invalidos, como por exemplo, espaços...</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -937,8 +1008,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G106" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G106"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G117" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G117"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1206,7 +1277,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1214,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G106"/>
+  <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,7 +1362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -1451,7 +1522,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>2</v>
       </c>
@@ -1491,7 +1562,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>2</v>
       </c>
@@ -1511,7 +1582,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>2</v>
       </c>
@@ -1531,7 +1602,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>2</v>
       </c>
@@ -1551,7 +1622,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>2</v>
       </c>
@@ -1571,7 +1642,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>2</v>
       </c>
@@ -1627,7 +1698,7 @@
       </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>2</v>
       </c>
@@ -1899,7 +1970,7 @@
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>2</v>
       </c>
@@ -1957,7 +2028,7 @@
       </c>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>2</v>
       </c>
@@ -1975,7 +2046,7 @@
       </c>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="2:7" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>2</v>
       </c>
@@ -1993,7 +2064,7 @@
       </c>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>2</v>
       </c>
@@ -2011,7 +2082,7 @@
       </c>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>2</v>
       </c>
@@ -2029,7 +2100,7 @@
       </c>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <v>2</v>
       </c>
@@ -2101,7 +2172,7 @@
       </c>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <v>2</v>
       </c>
@@ -2119,7 +2190,7 @@
       </c>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>2</v>
       </c>
@@ -2155,7 +2226,7 @@
       </c>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
         <v>2</v>
       </c>
@@ -2209,7 +2280,7 @@
       </c>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
         <v>2</v>
       </c>
@@ -2389,7 +2460,7 @@
       </c>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
         <v>2</v>
       </c>
@@ -2461,7 +2532,7 @@
       </c>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="1">
         <v>3</v>
       </c>
@@ -2604,7 +2675,7 @@
       </c>
       <c r="G74" s="3"/>
     </row>
-    <row r="75" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="8">
         <v>3</v>
       </c>
@@ -2696,7 +2767,7 @@
       </c>
       <c r="G79" s="3"/>
     </row>
-    <row r="80" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="1">
         <v>3</v>
       </c>
@@ -2734,7 +2805,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" s="1">
         <v>3</v>
       </c>
@@ -2862,7 +2933,7 @@
       </c>
       <c r="G88" s="10"/>
     </row>
-    <row r="89" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="8">
         <v>3</v>
       </c>
@@ -3012,7 +3083,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="97" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B97" s="8">
         <v>3</v>
       </c>
@@ -3086,7 +3157,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B101" s="8">
         <v>3</v>
       </c>
@@ -3115,12 +3186,14 @@
         <v>48</v>
       </c>
       <c r="E102" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F102" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F102" s="9"/>
       <c r="G102" s="10"/>
     </row>
-    <row r="103" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" s="8">
         <v>3</v>
       </c>
@@ -3131,10 +3204,10 @@
         <v>49</v>
       </c>
       <c r="E103" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F103" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>123</v>
       </c>
       <c r="G103" s="10"/>
     </row>
@@ -3149,9 +3222,11 @@
         <v>49</v>
       </c>
       <c r="E104" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F104" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="F104" s="9"/>
       <c r="G104" s="10"/>
     </row>
     <row r="105" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -3165,9 +3240,11 @@
         <v>49</v>
       </c>
       <c r="E105" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F105" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="F105" s="9"/>
       <c r="G105" s="10"/>
     </row>
     <row r="106" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -3181,10 +3258,214 @@
         <v>49</v>
       </c>
       <c r="E106" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F106" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F106" s="9"/>
       <c r="G106" s="10"/>
+    </row>
+    <row r="107" spans="2:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="B107" s="8">
+        <v>3</v>
+      </c>
+      <c r="C107" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D107" s="8">
+        <v>50</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G107" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B108" s="8">
+        <v>3</v>
+      </c>
+      <c r="C108" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D108" s="8">
+        <v>50</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G108" s="10"/>
+    </row>
+    <row r="109" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B109" s="8">
+        <v>3</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D109" s="8">
+        <v>50</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F109" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G109" s="10"/>
+    </row>
+    <row r="110" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B110" s="8">
+        <v>3</v>
+      </c>
+      <c r="C110" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D110" s="8">
+        <v>50</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G110" s="10"/>
+    </row>
+    <row r="111" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B111" s="8">
+        <v>3</v>
+      </c>
+      <c r="C111" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D111" s="8">
+        <v>50</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F111" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G111" s="10"/>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B112" s="8">
+        <v>3</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D112" s="8">
+        <v>50</v>
+      </c>
+      <c r="E112" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="G112" s="10"/>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B113" s="8">
+        <v>3</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D113" s="8">
+        <v>50</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="G113" s="10"/>
+    </row>
+    <row r="114" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B114" s="8">
+        <v>3</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D114" s="8">
+        <v>50</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G114" s="10"/>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B115" s="8">
+        <v>3</v>
+      </c>
+      <c r="C115" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D115" s="8">
+        <v>50</v>
+      </c>
+      <c r="E115" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G115" s="10"/>
+    </row>
+    <row r="116" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B116" s="8">
+        <v>3</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D116" s="8">
+        <v>51</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G116" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B117" s="1">
+        <v>3</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D117" s="1">
+        <v>51</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="G117" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Subtotal e total do Pedido
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="8430"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="187">
   <si>
     <t>nome aula</t>
   </si>
@@ -787,6 +787,12 @@
   </si>
   <si>
     <t>1:52 - criação de metodo de encode - que formata a URL eliminando caracteres invalidos, como por exemplo, espaços...</t>
+  </si>
+  <si>
+    <t>Subtotal e total do Pedido</t>
+  </si>
+  <si>
+    <t>nada de muito importanto, apenas criado 2 metods (getSubTotal e getValorTotal) nas classes Pedido e ItemPedido</t>
   </si>
 </sst>
 </file>
@@ -1008,8 +1014,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G117" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G117"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G118" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G118"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1285,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G117"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A113" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F117" sqref="F117"/>
+      <selection activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3467,6 +3473,24 @@
       </c>
       <c r="G117" s="3"/>
     </row>
+    <row r="118" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B118" s="8">
+        <v>3</v>
+      </c>
+      <c r="C118" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D118" s="8">
+        <v>52</v>
+      </c>
+      <c r="E118" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F118" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G118" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Criando profile de teste
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18045" windowHeight="8430"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="199">
   <si>
     <t>nome aula</t>
   </si>
@@ -845,6 +845,16 @@
       </rPr>
       <t>- aprendido como associar pedidos e produtos aos itensPedido</t>
     </r>
+  </si>
+  <si>
+    <t>3:49 - anotação @Profile em conjunto da anotação @Configuration - utilizada para criação da classe TestConfig, onde todas as injeçoes de depenncias foram retiradas da classe principal e transferidas para a classe DBService e depois instanciada na classe TestConfig ... este procedimento foi feito para que fosse criado um ambiente de testes da aplicação.</t>
+  </si>
+  <si>
+    <t>Banco de dados MySQL e Implantação no Heroku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Criando o profile de teste</t>
   </si>
 </sst>
 </file>
@@ -1073,8 +1083,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G126" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G126"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G127" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G127"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1350,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F124" sqref="F124"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3696,6 +3706,24 @@
       </c>
       <c r="G126" s="10"/>
     </row>
+    <row r="127" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B127" s="8">
+        <v>4</v>
+      </c>
+      <c r="C127" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D127" s="8">
+        <v>56</v>
+      </c>
+      <c r="E127" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="F127" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="G127" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Criando o profile de desenvolvimento
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18045" windowHeight="8430"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="202">
   <si>
     <t>nome aula</t>
   </si>
@@ -856,6 +856,15 @@
     <t xml:space="preserve">
 Criando o profile de teste</t>
   </si>
+  <si>
+    <t>Criando o profile de desenvolvimento</t>
+  </si>
+  <si>
+    <t>2:30 - ATENÇÃO - a tag spring.datasource.url nao funcionou no modo original da aula, tive que inserir ?serverTimezone=America/Sao_Paulo para que funcionasse corretamente</t>
+  </si>
+  <si>
+    <t>7:39 - anotação @Value("${spring.jpa.hibernate.ddl-auto}") - serve para captar o valor da chave de arquivos ".properties" .. no caso o arquivo de configuração do ambiente dev</t>
+  </si>
 </sst>
 </file>
 
@@ -960,42 +969,6 @@
   <dxfs count="8">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Consolas"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Consolas"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Consolas"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1010,6 +983,7 @@
         <name val="Consolas"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1055,6 +1029,42 @@
         <name val="Consolas"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Consolas"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Consolas"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Consolas"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1083,15 +1093,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G127" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G127"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G129" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G129"/>
   <tableColumns count="6">
-    <tableColumn id="5" name="Seção" dataDxfId="5"/>
-    <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
-    <tableColumn id="6" name="Aula" dataDxfId="3"/>
-    <tableColumn id="2" name="nome aula" dataDxfId="2"/>
-    <tableColumn id="3" name="abordagem da aula" dataDxfId="1"/>
-    <tableColumn id="4" name="aprendido" dataDxfId="0"/>
+    <tableColumn id="5" name="Seção" dataDxfId="2"/>
+    <tableColumn id="1" name="Nome da Seção" dataDxfId="0"/>
+    <tableColumn id="6" name="Aula" dataDxfId="1"/>
+    <tableColumn id="2" name="nome aula" dataDxfId="5"/>
+    <tableColumn id="3" name="abordagem da aula" dataDxfId="4"/>
+    <tableColumn id="4" name="aprendido" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1360,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G127"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A120" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E125" sqref="E125"/>
+      <selection activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,7 +1411,7 @@
       <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D2" s="1">
@@ -1421,7 +1431,7 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D3" s="1">
@@ -1441,7 +1451,7 @@
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D4" s="1">
@@ -1461,7 +1471,7 @@
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D5" s="1">
@@ -1481,7 +1491,7 @@
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D6" s="1">
@@ -1501,7 +1511,7 @@
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D7" s="1">
@@ -1521,7 +1531,7 @@
       <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D8" s="1">
@@ -1541,7 +1551,7 @@
       <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D9" s="1">
@@ -1561,7 +1571,7 @@
       <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D10" s="1">
@@ -1581,7 +1591,7 @@
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D11" s="1">
@@ -1601,7 +1611,7 @@
       <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D12" s="1">
@@ -1621,7 +1631,7 @@
       <c r="B13" s="1">
         <v>2</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D13" s="1">
@@ -1641,7 +1651,7 @@
       <c r="B14" s="1">
         <v>2</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D14" s="1">
@@ -1661,7 +1671,7 @@
       <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D15" s="1">
@@ -1681,7 +1691,7 @@
       <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D16" s="1">
@@ -1701,7 +1711,7 @@
       <c r="B17" s="1">
         <v>2</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D17" s="1">
@@ -1721,7 +1731,7 @@
       <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D18" s="1">
@@ -1741,7 +1751,7 @@
       <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D19" s="1">
@@ -1759,7 +1769,7 @@
       <c r="B20" s="1">
         <v>2</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D20" s="1">
@@ -1777,7 +1787,7 @@
       <c r="B21" s="1">
         <v>2</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D21" s="1">
@@ -1795,7 +1805,7 @@
       <c r="B22" s="1">
         <v>2</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D22" s="1">
@@ -1813,7 +1823,7 @@
       <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D23" s="1">
@@ -1831,7 +1841,7 @@
       <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D24" s="1">
@@ -1849,7 +1859,7 @@
       <c r="B25" s="1">
         <v>2</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D25" s="1">
@@ -1867,7 +1877,7 @@
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D26" s="1">
@@ -1885,7 +1895,7 @@
       <c r="B27" s="1">
         <v>2</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D27" s="1">
@@ -1903,7 +1913,7 @@
       <c r="B28" s="1">
         <v>2</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D28" s="1">
@@ -1921,7 +1931,7 @@
       <c r="B29" s="1">
         <v>2</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D29" s="1">
@@ -1939,7 +1949,7 @@
       <c r="B30" s="1">
         <v>2</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D30" s="1">
@@ -1957,7 +1967,7 @@
       <c r="B31" s="1">
         <v>2</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D31" s="1">
@@ -1977,7 +1987,7 @@
       <c r="B32" s="1">
         <v>2</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D32" s="1">
@@ -1995,7 +2005,7 @@
       <c r="B33" s="1">
         <v>2</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D33" s="1">
@@ -2013,7 +2023,7 @@
       <c r="B34" s="1">
         <v>2</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D34" s="1">
@@ -2031,7 +2041,7 @@
       <c r="B35" s="1">
         <v>2</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D35" s="1">
@@ -2049,7 +2059,7 @@
       <c r="B36" s="1">
         <v>2</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D36" s="1">
@@ -2069,7 +2079,7 @@
       <c r="B37" s="1">
         <v>2</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D37" s="1">
@@ -2089,7 +2099,7 @@
       <c r="B38" s="1">
         <v>2</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D38" s="1">
@@ -2107,7 +2117,7 @@
       <c r="B39" s="1">
         <v>2</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D39" s="1">
@@ -2125,7 +2135,7 @@
       <c r="B40" s="1">
         <v>2</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D40" s="2">
@@ -2143,7 +2153,7 @@
       <c r="B41" s="1">
         <v>2</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D41" s="2">
@@ -2161,7 +2171,7 @@
       <c r="B42" s="1">
         <v>2</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D42" s="2">
@@ -2179,7 +2189,7 @@
       <c r="B43" s="1">
         <v>2</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D43" s="2">
@@ -2197,7 +2207,7 @@
       <c r="B44" s="1">
         <v>2</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D44" s="2">
@@ -2215,7 +2225,7 @@
       <c r="B45" s="1">
         <v>2</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D45" s="2">
@@ -2233,7 +2243,7 @@
       <c r="B46" s="1">
         <v>2</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D46" s="1">
@@ -2251,7 +2261,7 @@
       <c r="B47" s="1">
         <v>2</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D47" s="1">
@@ -2269,7 +2279,7 @@
       <c r="B48" s="1">
         <v>2</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D48" s="1">
@@ -2287,7 +2297,7 @@
       <c r="B49" s="1">
         <v>2</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D49" s="1">
@@ -2305,7 +2315,7 @@
       <c r="B50" s="1">
         <v>2</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D50" s="1">
@@ -2323,7 +2333,7 @@
       <c r="B51" s="1">
         <v>2</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D51" s="1">
@@ -2341,7 +2351,7 @@
       <c r="B52" s="1">
         <v>2</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D52" s="1">
@@ -2359,7 +2369,7 @@
       <c r="B53" s="1">
         <v>2</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D53" s="1">
@@ -2377,7 +2387,7 @@
       <c r="B54" s="1">
         <v>2</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D54" s="1">
@@ -2395,7 +2405,7 @@
       <c r="B55" s="1">
         <v>2</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D55" s="1">
@@ -2413,7 +2423,7 @@
       <c r="B56" s="1">
         <v>2</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D56" s="1">
@@ -2431,7 +2441,7 @@
       <c r="B57" s="1">
         <v>2</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D57" s="1">
@@ -2449,7 +2459,7 @@
       <c r="B58" s="1">
         <v>2</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D58" s="1">
@@ -2467,7 +2477,7 @@
       <c r="B59" s="1">
         <v>2</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D59" s="1">
@@ -2485,7 +2495,7 @@
       <c r="B60" s="1">
         <v>2</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D60" s="1">
@@ -2503,7 +2513,7 @@
       <c r="B61" s="1">
         <v>2</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D61" s="1">
@@ -2521,7 +2531,7 @@
       <c r="B62" s="1">
         <v>2</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D62" s="1">
@@ -2539,7 +2549,7 @@
       <c r="B63" s="1">
         <v>2</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D63" s="1">
@@ -2557,7 +2567,7 @@
       <c r="B64" s="1">
         <v>2</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D64" s="1">
@@ -2575,7 +2585,7 @@
       <c r="B65" s="1">
         <v>2</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="2" t="s">
         <v>130</v>
       </c>
       <c r="D65" s="1">
@@ -2593,7 +2603,7 @@
       <c r="B66" s="6">
         <v>2</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="7" t="s">
         <v>130</v>
       </c>
       <c r="D66" s="6">
@@ -2611,7 +2621,7 @@
       <c r="B67" s="1">
         <v>3</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D67" s="1">
@@ -2626,7 +2636,7 @@
       <c r="B68" s="1">
         <v>3</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D68" s="1">
@@ -2646,7 +2656,7 @@
       <c r="B69" s="1">
         <v>3</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D69" s="1">
@@ -2664,7 +2674,7 @@
       <c r="B70" s="1">
         <v>3</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D70" s="1">
@@ -2682,7 +2692,7 @@
       <c r="B71" s="1">
         <v>3</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D71" s="1">
@@ -2700,7 +2710,7 @@
       <c r="B72" s="1">
         <v>3</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D72" s="1">
@@ -2718,7 +2728,7 @@
       <c r="B73" s="1">
         <v>3</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D73" s="1">
@@ -2736,7 +2746,7 @@
       <c r="B74" s="1">
         <v>3</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D74" s="1">
@@ -2754,7 +2764,7 @@
       <c r="B75" s="8">
         <v>3</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D75" s="8">
@@ -2772,7 +2782,7 @@
       <c r="B76" s="8">
         <v>3</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D76" s="8">
@@ -2790,7 +2800,7 @@
       <c r="B77" s="8">
         <v>3</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D77" s="8">
@@ -2808,7 +2818,7 @@
       <c r="B78" s="1">
         <v>3</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D78" s="1">
@@ -2828,7 +2838,7 @@
       <c r="B79" s="1">
         <v>3</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D79" s="1">
@@ -2846,7 +2856,7 @@
       <c r="B80" s="1">
         <v>3</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D80" s="1">
@@ -2864,7 +2874,7 @@
       <c r="B81" s="1">
         <v>3</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D81" s="1">
@@ -2884,7 +2894,7 @@
       <c r="B82" s="1">
         <v>3</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D82" s="1">
@@ -2902,7 +2912,7 @@
       <c r="B83" s="1">
         <v>3</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D83" s="1">
@@ -2920,7 +2930,7 @@
       <c r="B84" s="1">
         <v>3</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D84" s="1">
@@ -2938,7 +2948,7 @@
       <c r="B85" s="8">
         <v>3</v>
       </c>
-      <c r="C85" s="8" t="s">
+      <c r="C85" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D85" s="8">
@@ -2958,7 +2968,7 @@
       <c r="B86" s="8">
         <v>3</v>
       </c>
-      <c r="C86" s="8" t="s">
+      <c r="C86" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D86" s="8">
@@ -2976,7 +2986,7 @@
       <c r="B87" s="8">
         <v>3</v>
       </c>
-      <c r="C87" s="8" t="s">
+      <c r="C87" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D87" s="8">
@@ -2994,7 +3004,7 @@
       <c r="B88" s="8">
         <v>3</v>
       </c>
-      <c r="C88" s="8" t="s">
+      <c r="C88" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D88" s="8">
@@ -3012,7 +3022,7 @@
       <c r="B89" s="8">
         <v>3</v>
       </c>
-      <c r="C89" s="8" t="s">
+      <c r="C89" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D89" s="8">
@@ -3030,7 +3040,7 @@
       <c r="B90" s="8">
         <v>3</v>
       </c>
-      <c r="C90" s="8" t="s">
+      <c r="C90" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D90" s="8">
@@ -3048,7 +3058,7 @@
       <c r="B91" s="8">
         <v>3</v>
       </c>
-      <c r="C91" s="8" t="s">
+      <c r="C91" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D91" s="8">
@@ -3066,7 +3076,7 @@
       <c r="B92" s="8">
         <v>3</v>
       </c>
-      <c r="C92" s="8" t="s">
+      <c r="C92" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D92" s="8">
@@ -3086,7 +3096,7 @@
       <c r="B93" s="8">
         <v>3</v>
       </c>
-      <c r="C93" s="8" t="s">
+      <c r="C93" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D93" s="8">
@@ -3104,7 +3114,7 @@
       <c r="B94" s="8">
         <v>3</v>
       </c>
-      <c r="C94" s="8" t="s">
+      <c r="C94" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D94" s="8">
@@ -3124,7 +3134,7 @@
       <c r="B95" s="8">
         <v>3</v>
       </c>
-      <c r="C95" s="8" t="s">
+      <c r="C95" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D95" s="8">
@@ -3142,7 +3152,7 @@
       <c r="B96" s="8">
         <v>3</v>
       </c>
-      <c r="C96" s="8" t="s">
+      <c r="C96" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D96" s="8">
@@ -3162,7 +3172,7 @@
       <c r="B97" s="8">
         <v>3</v>
       </c>
-      <c r="C97" s="8" t="s">
+      <c r="C97" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D97" s="8">
@@ -3180,7 +3190,7 @@
       <c r="B98" s="8">
         <v>3</v>
       </c>
-      <c r="C98" s="8" t="s">
+      <c r="C98" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D98" s="8">
@@ -3198,7 +3208,7 @@
       <c r="B99" s="8">
         <v>3</v>
       </c>
-      <c r="C99" s="8" t="s">
+      <c r="C99" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D99" s="8">
@@ -3216,7 +3226,7 @@
       <c r="B100" s="8">
         <v>3</v>
       </c>
-      <c r="C100" s="8" t="s">
+      <c r="C100" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D100" s="8">
@@ -3236,7 +3246,7 @@
       <c r="B101" s="8">
         <v>3</v>
       </c>
-      <c r="C101" s="8" t="s">
+      <c r="C101" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D101" s="8">
@@ -3254,7 +3264,7 @@
       <c r="B102" s="8">
         <v>3</v>
       </c>
-      <c r="C102" s="8" t="s">
+      <c r="C102" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D102" s="8">
@@ -3272,7 +3282,7 @@
       <c r="B103" s="8">
         <v>3</v>
       </c>
-      <c r="C103" s="8" t="s">
+      <c r="C103" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D103" s="8">
@@ -3290,7 +3300,7 @@
       <c r="B104" s="8">
         <v>3</v>
       </c>
-      <c r="C104" s="8" t="s">
+      <c r="C104" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D104" s="8">
@@ -3308,7 +3318,7 @@
       <c r="B105" s="8">
         <v>3</v>
       </c>
-      <c r="C105" s="8" t="s">
+      <c r="C105" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D105" s="8">
@@ -3326,7 +3336,7 @@
       <c r="B106" s="8">
         <v>3</v>
       </c>
-      <c r="C106" s="8" t="s">
+      <c r="C106" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D106" s="8">
@@ -3344,7 +3354,7 @@
       <c r="B107" s="8">
         <v>3</v>
       </c>
-      <c r="C107" s="8" t="s">
+      <c r="C107" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D107" s="8">
@@ -3364,7 +3374,7 @@
       <c r="B108" s="8">
         <v>3</v>
       </c>
-      <c r="C108" s="8" t="s">
+      <c r="C108" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D108" s="8">
@@ -3382,7 +3392,7 @@
       <c r="B109" s="8">
         <v>3</v>
       </c>
-      <c r="C109" s="8" t="s">
+      <c r="C109" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D109" s="8">
@@ -3400,7 +3410,7 @@
       <c r="B110" s="8">
         <v>3</v>
       </c>
-      <c r="C110" s="8" t="s">
+      <c r="C110" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D110" s="8">
@@ -3418,7 +3428,7 @@
       <c r="B111" s="8">
         <v>3</v>
       </c>
-      <c r="C111" s="8" t="s">
+      <c r="C111" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D111" s="8">
@@ -3436,7 +3446,7 @@
       <c r="B112" s="8">
         <v>3</v>
       </c>
-      <c r="C112" s="8" t="s">
+      <c r="C112" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D112" s="8">
@@ -3454,7 +3464,7 @@
       <c r="B113" s="8">
         <v>3</v>
       </c>
-      <c r="C113" s="8" t="s">
+      <c r="C113" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D113" s="8">
@@ -3472,7 +3482,7 @@
       <c r="B114" s="8">
         <v>3</v>
       </c>
-      <c r="C114" s="8" t="s">
+      <c r="C114" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D114" s="8">
@@ -3490,7 +3500,7 @@
       <c r="B115" s="8">
         <v>3</v>
       </c>
-      <c r="C115" s="8" t="s">
+      <c r="C115" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D115" s="8">
@@ -3508,7 +3518,7 @@
       <c r="B116" s="8">
         <v>3</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D116" s="8">
@@ -3528,7 +3538,7 @@
       <c r="B117" s="1">
         <v>3</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="2" t="s">
         <v>125</v>
       </c>
       <c r="D117" s="1">
@@ -3546,7 +3556,7 @@
       <c r="B118" s="8">
         <v>3</v>
       </c>
-      <c r="C118" s="8" t="s">
+      <c r="C118" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D118" s="8">
@@ -3564,7 +3574,7 @@
       <c r="B119" s="8">
         <v>3</v>
       </c>
-      <c r="C119" s="8" t="s">
+      <c r="C119" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D119" s="8">
@@ -3584,7 +3594,7 @@
       <c r="B120" s="8">
         <v>3</v>
       </c>
-      <c r="C120" s="8" t="s">
+      <c r="C120" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D120" s="8">
@@ -3602,7 +3612,7 @@
       <c r="B121" s="8">
         <v>3</v>
       </c>
-      <c r="C121" s="8" t="s">
+      <c r="C121" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D121" s="8">
@@ -3620,7 +3630,7 @@
       <c r="B122" s="8">
         <v>3</v>
       </c>
-      <c r="C122" s="8" t="s">
+      <c r="C122" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D122" s="8">
@@ -3638,7 +3648,7 @@
       <c r="B123" s="8">
         <v>3</v>
       </c>
-      <c r="C123" s="8" t="s">
+      <c r="C123" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D123" s="8">
@@ -3656,7 +3666,7 @@
       <c r="B124" s="8">
         <v>3</v>
       </c>
-      <c r="C124" s="8" t="s">
+      <c r="C124" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D124" s="8">
@@ -3674,7 +3684,7 @@
       <c r="B125" s="8">
         <v>3</v>
       </c>
-      <c r="C125" s="8" t="s">
+      <c r="C125" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D125" s="8">
@@ -3692,7 +3702,7 @@
       <c r="B126" s="8">
         <v>3</v>
       </c>
-      <c r="C126" s="8" t="s">
+      <c r="C126" s="9" t="s">
         <v>125</v>
       </c>
       <c r="D126" s="8">
@@ -3723,6 +3733,44 @@
         <v>196</v>
       </c>
       <c r="G127" s="10"/>
+    </row>
+    <row r="128" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B128" s="8">
+        <v>4</v>
+      </c>
+      <c r="C128" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D128" s="8">
+        <v>57</v>
+      </c>
+      <c r="E128" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F128" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="G128" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B129" s="8">
+        <v>4</v>
+      </c>
+      <c r="C129" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D129" s="8">
+        <v>57</v>
+      </c>
+      <c r="E129" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F129" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G129" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Configuracao e envio do projeto para producao
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18045" windowHeight="5580"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="207">
   <si>
     <t>nome aula</t>
   </si>
@@ -865,6 +865,31 @@
   <si>
     <t>7:39 - anotação @Value("${spring.jpa.hibernate.ddl-auto}") - serve para captar o valor da chave de arquivos ".properties" .. no caso o arquivo de configuração do ambiente dev</t>
   </si>
+  <si>
+    <t>Instalando e preparando o Heroku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:38 - fazer login no heroku CLI pelo terminaol cmd do windows -
+abrir CMD e digitar "heroku login" sem aspas
+vai pedir o login e senha da conta do heroku
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+2:28 - instalação do software "Heroku CLI" no computador - programa que permite logar no heroku e efetuar operações remotas na aplicação</t>
+  </si>
+  <si>
+    <t>1:30 - instalação do MySQL no heroku - adiciona uma instancia do MySQL ... necessário inserir um cartao de crédito
+aba Overview-&gt;Configure Add-ons
+pesquisar por "MySQL" e escolher o ClearDB MySQL
+Escolher um plano e clocar em "Provide"</t>
+  </si>
+  <si>
+    <t>0:50 - procedimento de criar app novo no heroku -
+Creatre new app
+nome do app (opcional)
+localidade (pais)</t>
+  </si>
 </sst>
 </file>
 
@@ -969,17 +994,35 @@
   <dxfs count="8">
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
+        <name val="Consolas"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Consolas"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
         <name val="Consolas"/>
         <scheme val="none"/>
       </font>
@@ -1018,42 +1061,24 @@
         <name val="Consolas"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
         <name val="Consolas"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Consolas"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Consolas"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1093,15 +1118,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G129" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G129"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G133" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G133"/>
   <tableColumns count="6">
-    <tableColumn id="5" name="Seção" dataDxfId="2"/>
-    <tableColumn id="1" name="Nome da Seção" dataDxfId="0"/>
-    <tableColumn id="6" name="Aula" dataDxfId="1"/>
-    <tableColumn id="2" name="nome aula" dataDxfId="5"/>
-    <tableColumn id="3" name="abordagem da aula" dataDxfId="4"/>
-    <tableColumn id="4" name="aprendido" dataDxfId="3"/>
+    <tableColumn id="5" name="Seção" dataDxfId="5"/>
+    <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
+    <tableColumn id="6" name="Aula" dataDxfId="3"/>
+    <tableColumn id="2" name="nome aula" dataDxfId="2"/>
+    <tableColumn id="3" name="abordagem da aula" dataDxfId="1"/>
+    <tableColumn id="4" name="aprendido" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1370,10 +1395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G129"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F128" sqref="F128"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3772,6 +3797,80 @@
       </c>
       <c r="G129" s="10"/>
     </row>
+    <row r="130" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B130" s="8">
+        <v>4</v>
+      </c>
+      <c r="C130" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D130" s="8">
+        <v>58</v>
+      </c>
+      <c r="E130" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F130" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="G130" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B131" s="8">
+        <v>4</v>
+      </c>
+      <c r="C131" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D131" s="8">
+        <v>58</v>
+      </c>
+      <c r="E131" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F131" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G131" s="10"/>
+    </row>
+    <row r="132" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B132" s="8">
+        <v>4</v>
+      </c>
+      <c r="C132" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D132" s="8">
+        <v>58</v>
+      </c>
+      <c r="E132" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F132" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="G132" s="10"/>
+    </row>
+    <row r="133" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B133" s="8">
+        <v>4</v>
+      </c>
+      <c r="C133" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D133" s="8">
+        <v>58</v>
+      </c>
+      <c r="E133" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F133" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G133" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementando toString de Pedido
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\CURSO - SPRING BOOT, IONIC\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18045" windowHeight="5580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="230">
   <si>
     <t>nome aula</t>
   </si>
@@ -992,6 +988,41 @@
   </si>
   <si>
     <t>Configuração e envio do projeto para produção</t>
+  </si>
+  <si>
+    <t>4:30
+5. Serviço de email
+62. Implementando toString de Pedido
+implementa toString no mode String build/String Buffer - para ser mais performatico</t>
+  </si>
+  <si>
+    <t>10:57
+5. Serviço de email
+62. Implementando toString de Pedido
+ATUALIZAÇÂO - no video descreve a utilização do ClienteRepository mas lembrar que no inicia há uma atualização indicando para usar ClienteService para simplificar</t>
+  </si>
+  <si>
+    <t>12:29
+5. Serviço de email
+62. Implementando toString de Pedido
+NumberFormat - NumberFormat nf = NumberFormat.getCurrencyInstance(new Locale("pt","BR")); ..formata valores monetarios para a moeda brasileira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14:06
+5. Serviço de email
+62. Implementando toString de Pedido
+formata data com SimpleDateFormat - SimpleDateFormat sdf = new SimpleDateFormat("dd/MM/yyyy hh:mm:ss");
+</t>
+  </si>
+  <si>
+    <t>Serviço de email</t>
+  </si>
+  <si>
+    <t>Implementando toString de Pedido</t>
   </si>
 </sst>
 </file>
@@ -1221,8 +1252,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G145" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G145"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G149" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G149"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1498,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G145"/>
+  <dimension ref="A1:G149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E142" sqref="E142"/>
+    <sheetView tabSelected="1" topLeftCell="B143" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E150" sqref="E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,7 +1586,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="150" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>2</v>
       </c>
@@ -1715,7 +1746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -1735,7 +1766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>2</v>
       </c>
@@ -1755,7 +1786,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>2</v>
       </c>
@@ -1795,7 +1826,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>2</v>
       </c>
@@ -2091,7 +2122,7 @@
       </c>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="2:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" ht="408.75" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>2</v>
       </c>
@@ -2760,7 +2791,7 @@
       </c>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B68" s="1">
         <v>3</v>
       </c>
@@ -4193,6 +4224,80 @@
         <v>221</v>
       </c>
       <c r="G145" s="10"/>
+    </row>
+    <row r="146" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B146" s="8">
+        <v>5</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D146" s="8">
+        <v>62</v>
+      </c>
+      <c r="E146" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F146" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="G146" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="147" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B147" s="8">
+        <v>5</v>
+      </c>
+      <c r="C147" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D147" s="8">
+        <v>62</v>
+      </c>
+      <c r="E147" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F147" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="G147" s="10"/>
+    </row>
+    <row r="148" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B148" s="8">
+        <v>5</v>
+      </c>
+      <c r="C148" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D148" s="8">
+        <v>62</v>
+      </c>
+      <c r="E148" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F148" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="G148" s="10"/>
+    </row>
+    <row r="149" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B149" s="8">
+        <v>5</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D149" s="8">
+        <v>62</v>
+      </c>
+      <c r="E149" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F149" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="G149" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
MockEmailService com Logger. Padroes Strategy e Template Method
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="236">
   <si>
     <t>nome aula</t>
   </si>
@@ -1023,6 +1023,39 @@
   </si>
   <si>
     <t>Implementando toString de Pedido</t>
+  </si>
+  <si>
+    <t>1:57
+5. Serviço de email
+63. MockEmailService com Logger. Padroes Strategy e Template Method
+padrão de projeto "Strategy" - polimorfismo</t>
+  </si>
+  <si>
+    <t>3:48
+5. Serviço de email
+63. MockEmailService com Logger. Padroes Strategy e Template Method
+padrao de projeto "Template Method"</t>
+  </si>
+  <si>
+    <t>9:23
+5. Serviço de email
+63. MockEmailService com Logger. Padroes Strategy e Template Method
+criação do MockMailService - email de mentirinha no log do servidor</t>
+  </si>
+  <si>
+    <t>9:56
+5. Serviço de email
+63. MockEmailService com Logger. Padroes Strategy e Template Method
+instancia um objeto de Logger</t>
+  </si>
+  <si>
+    <t>12:29
+5. Serviço de email
+63. MockEmailService com Logger. Padroes Strategy e Template Method
+criação de metodo @Bean de test na classe TestConfig - retornando um MockemailService</t>
+  </si>
+  <si>
+    <t>MockEmailService com Logger. Padroes Strategy e Template Method</t>
   </si>
 </sst>
 </file>
@@ -1252,8 +1285,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G149" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G149"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G154" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G154"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1529,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G149"/>
+  <dimension ref="A1:G154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B143" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E150" sqref="E150"/>
+    <sheetView tabSelected="1" topLeftCell="B149" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4299,6 +4332,98 @@
       </c>
       <c r="G149" s="10"/>
     </row>
+    <row r="150" spans="2:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="B150" s="8">
+        <v>5</v>
+      </c>
+      <c r="C150" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D150" s="8">
+        <v>63</v>
+      </c>
+      <c r="E150" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F150" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="G150" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="151" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B151" s="8">
+        <v>5</v>
+      </c>
+      <c r="C151" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D151" s="8">
+        <v>63</v>
+      </c>
+      <c r="E151" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F151" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G151" s="10"/>
+    </row>
+    <row r="152" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B152" s="8">
+        <v>5</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D152" s="8">
+        <v>63</v>
+      </c>
+      <c r="E152" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F152" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="G152" s="10"/>
+    </row>
+    <row r="153" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B153" s="8">
+        <v>5</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D153" s="8">
+        <v>63</v>
+      </c>
+      <c r="E153" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F153" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="G153" s="10"/>
+    </row>
+    <row r="154" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B154" s="8">
+        <v>5</v>
+      </c>
+      <c r="C154" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D154" s="8">
+        <v>63</v>
+      </c>
+      <c r="E154" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F154" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="G154" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementando SmtpEmailService com servidor do Google
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="241">
   <si>
     <t>nome aula</t>
   </si>
@@ -1056,6 +1056,33 @@
   </si>
   <si>
     <t>MockEmailService com Logger. Padroes Strategy e Template Method</t>
+  </si>
+  <si>
+    <t>4:22
+5. Serviço de email
+64. Implementando SmtpEmailService com servidor do Google
+instanciação de MailSender que é uma classe do framework - ele automaticamente pega os dados de e-mail do arquivo application.properties para enviar e-mails</t>
+  </si>
+  <si>
+    <t>5:18
+5. Serviço de email
+64. Implementando SmtpEmailService com servidor do Google
+criação da classe SmtpEmailService - responsável por pegar os dados de configs de login e senha do arquivo application.properties e enviar e-mails</t>
+  </si>
+  <si>
+    <t>7:06
+5. Serviço de email
+64. Implementando SmtpEmailService com servidor do Google
+criação de @Bean na classe DevConfig para instanciação de SmtpEmailService (envio de e-mail)</t>
+  </si>
+  <si>
+    <t>8:36
+5. Serviço de email
+64. Implementando SmtpEmailService com servidor do Google
+IMPORTANTE: o envio de e-mail (PELO GOGGLE SMTP) só funcionou para mim utilizando a solução descrita na aula (acessando a aba Segurança&gt;Acesso a app menos seguro&gt;ATIVAR ou pelo link https://myaccount.google.com/lesssecureapps) porém foi necessário também desativar o antivirus temporariamente</t>
+  </si>
+  <si>
+    <t>Implementando SmtpEmailService com servidor do Google</t>
   </si>
 </sst>
 </file>
@@ -1285,8 +1312,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G154" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G154"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G158" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G158"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1562,10 +1589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G154"/>
+  <dimension ref="A1:G158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B149" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView tabSelected="1" topLeftCell="B144" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4424,6 +4451,80 @@
       </c>
       <c r="G154" s="10"/>
     </row>
+    <row r="155" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B155" s="8">
+        <v>5</v>
+      </c>
+      <c r="C155" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D155" s="8">
+        <v>64</v>
+      </c>
+      <c r="E155" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F155" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="G155" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="156" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B156" s="8">
+        <v>5</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D156" s="8">
+        <v>64</v>
+      </c>
+      <c r="E156" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F156" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="G156" s="10"/>
+    </row>
+    <row r="157" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B157" s="8">
+        <v>5</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D157" s="8">
+        <v>64</v>
+      </c>
+      <c r="E157" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F157" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="G157" s="10"/>
+    </row>
+    <row r="158" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="B158" s="8">
+        <v>5</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D158" s="8">
+        <v>64</v>
+      </c>
+      <c r="E158" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="F158" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G158" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
commit sem ligacao com a aula - corrigindo arquivos application.properties e atualizacao da planilha de anotaçoes
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="243">
   <si>
     <t>nome aula</t>
   </si>
@@ -1076,20 +1076,94 @@
 criação de @Bean na classe DevConfig para instanciação de SmtpEmailService (envio de e-mail)</t>
   </si>
   <si>
-    <t>8:36
+    <t>Implementando SmtpEmailService com servidor do Google</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8:36
 5. Serviço de email
 64. Implementando SmtpEmailService com servidor do Google
-IMPORTANTE: o envio de e-mail (PELO GOGGLE SMTP) só funcionou para mim utilizando a solução descrita na aula (acessando a aba Segurança&gt;Acesso a app menos seguro&gt;ATIVAR ou pelo link https://myaccount.google.com/lesssecureapps) porém foi necessário também desativar o antivirus temporariamente</t>
-  </si>
-  <si>
-    <t>Implementando SmtpEmailService com servidor do Google</t>
+IMPORTANTE: o envio de e-mail (PELO GOGGLE SMTP) só funcionou para mim utilizando a solução descrita na aula (acessando a aba Segurança&gt;Acesso a app menos seguro&gt;ATIVAR ou pelo link </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>https://myaccount.google.com/lesssecureapps</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> )</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+      </rPr>
+      <t xml:space="preserve"> porém foi necessário também desativar o antivirus temporariamente</t>
+    </r>
+  </si>
+  <si>
+    <t>Atualização: outro link para liberar acesso ao Gmail</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">alem do link da aula para permitir acesso a conta google, no material de apoio existe este outro link, para permitir acesso por outros aplicativos e evitar bloqueio quando o app estiver na playstore.
+o link é: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">https://accounts.google.com/b/0/DisplayUnlockCaptcha
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Referência:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://stackoverflow.com/questions/25341198/javax-mail-authenticationfailedexception-is-thrown-while-sending-email-in-java/33801654</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1134,6 +1208,36 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1155,7 +1259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1180,6 +1284,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1312,8 +1419,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G158" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G158"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G159" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G159"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1589,10 +1696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G158"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B144" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E155" sqref="E155"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4462,7 +4569,7 @@
         <v>64</v>
       </c>
       <c r="E155" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F155" s="9" t="s">
         <v>236</v>
@@ -4482,7 +4589,7 @@
         <v>64</v>
       </c>
       <c r="E156" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F156" s="9" t="s">
         <v>237</v>
@@ -4500,7 +4607,7 @@
         <v>64</v>
       </c>
       <c r="E157" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F157" s="9" t="s">
         <v>238</v>
@@ -4518,12 +4625,30 @@
         <v>64</v>
       </c>
       <c r="E158" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="F158" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F158" s="9" t="s">
-        <v>239</v>
-      </c>
       <c r="G158" s="10"/>
+    </row>
+    <row r="159" spans="2:7" ht="189.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B159" s="1">
+        <v>5</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D159" s="1">
+        <v>65</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F159" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="G159" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Adicionando senha a Cliente
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18600" windowHeight="6675"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="260">
   <si>
     <t>nome aula</t>
   </si>
@@ -1189,6 +1189,79 @@
   </si>
   <si>
     <t>Email Html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+4:14
+6. Autenticação e autorização com tokens JWT
+68. Configuração inicial do Spring Security
+o simples fato de adicionar as dependencias do JWT ja bloqueia os endpoints
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+5:29
+6. Autenticação e autorização com tokens JWT
+68. Configuração inicial do Spring Security
+anotação @EnableWebSecurity do spring security
+</t>
+  </si>
+  <si>
+    <t>6:14
+6. Autenticação e autorização com tokens JWT
+68. Configuração inicial do Spring Security
+sobrescrever metodo protected void configure (HttpSecurity http)</t>
+  </si>
+  <si>
+    <t>7:13
+6. Autenticação e autorização com tokens JWT
+68. Configuração inicial do Spring Security
+define no metodo sobrescrito que todos os caminhos descritos no vetor (no caso endpoints) serão permitidos o acesso ... para todo os outros, será necessário autenticação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+9:02
+6. Autenticação e autorização com tokens JWT
+68. Configuração inicial do Spring Security
+configuração para o back end De modo geral pode-se desabilitar proteção de ataques a CSRF em sistemas stateless - nosso sistema é stateless, o que significa que nao armazena seção de usuário</t>
+  </si>
+  <si>
+    <t>9:51
+6. Autenticação e autorização com tokens JWT
+68. Configuração inicial do Spring Security
+o teste sugerido na aula não funcionou - para resolver foi necessário incluir um @Bean na classe JacksonConfig para funcionar com o profile de test e com o H2
+@Bean
+public JavaMailSender jms (){
+return new JavaMailSenderImpl();
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+3:15 - Adiciona dependencias necessarias para o JWT (Json Web Tokens) funcionar:
+&lt;dependency&gt;
+&lt;groupId&gt;org.springframework.boot&lt;/groupId&gt;
+&lt;artifactId&gt;spring-boot-starter-security&lt;/artifactId&gt;
+&lt;/dependency&gt;
+&lt;dependency&gt;
+&lt;groupId&gt;io.jsonwebtoken&lt;/groupId&gt;
+&lt;artifactId&gt;jjwt&lt;/artifactId&gt;
+&lt;version&gt;0.7.0&lt;/version&gt;
+&lt;/dependency&gt;</t>
+  </si>
+  <si>
+    <t>. Configuração inicial do Spring Security</t>
+  </si>
+  <si>
+    <t>Autenticação e autorização com tokens JWT</t>
+  </si>
+  <si>
+    <t>0:57
+6. Autenticação e autorização com tokens JWT
+69. Adicionando senha a Cliente
+Criação de @Bean de BCryptPasswordEncoder no arquivo de configuração - tem a função de criptografar a senha para armazenar no banco de dados</t>
+  </si>
+  <si>
+    <t>Adicionando senha a Cliente</t>
   </si>
 </sst>
 </file>
@@ -1451,8 +1524,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G164" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G164"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G172" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G172"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1728,10 +1801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G164"/>
+  <dimension ref="A1:G172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B159" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F161" sqref="F161"/>
+    <sheetView tabSelected="1" topLeftCell="B169" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C173" sqref="C173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4772,6 +4845,152 @@
       </c>
       <c r="G164" s="10"/>
     </row>
+    <row r="165" spans="2:7" ht="345" x14ac:dyDescent="0.25">
+      <c r="B165" s="8">
+        <v>6</v>
+      </c>
+      <c r="C165" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D165" s="8">
+        <v>68</v>
+      </c>
+      <c r="E165" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="F165" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="G165" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B166" s="8">
+        <v>6</v>
+      </c>
+      <c r="C166" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D166" s="8">
+        <v>68</v>
+      </c>
+      <c r="E166" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="F166" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="G166" s="10"/>
+    </row>
+    <row r="167" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B167" s="8">
+        <v>6</v>
+      </c>
+      <c r="C167" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D167" s="8">
+        <v>68</v>
+      </c>
+      <c r="E167" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="F167" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="G167" s="10"/>
+    </row>
+    <row r="168" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B168" s="8">
+        <v>6</v>
+      </c>
+      <c r="C168" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D168" s="8">
+        <v>68</v>
+      </c>
+      <c r="E168" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="F168" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="G168" s="10"/>
+    </row>
+    <row r="169" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B169" s="8">
+        <v>6</v>
+      </c>
+      <c r="C169" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D169" s="8">
+        <v>68</v>
+      </c>
+      <c r="E169" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="F169" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="G169" s="10"/>
+    </row>
+    <row r="170" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B170" s="8">
+        <v>6</v>
+      </c>
+      <c r="C170" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D170" s="8">
+        <v>68</v>
+      </c>
+      <c r="E170" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="F170" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="G170" s="10"/>
+    </row>
+    <row r="171" spans="2:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="B171" s="8">
+        <v>6</v>
+      </c>
+      <c r="C171" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D171" s="8">
+        <v>68</v>
+      </c>
+      <c r="E171" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="F171" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="G171" s="10"/>
+    </row>
+    <row r="172" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B172" s="8">
+        <v>6</v>
+      </c>
+      <c r="C172" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D172" s="8">
+        <v>69</v>
+      </c>
+      <c r="E172" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="F172" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="G172" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Salvando perfis de usuario na base de dados
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="264">
   <si>
     <t>nome aula</t>
   </si>
@@ -1262,6 +1262,28 @@
   </si>
   <si>
     <t>Adicionando senha a Cliente</t>
+  </si>
+  <si>
+    <t>0:31
+6. Autenticação e autorização com tokens JWT
+70. Salvando perfis de usuário na base de dados
+Criação de tipo enumerado "Perfil" - que tera função para definir os tipos de usuários</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1:07
+6. Autenticação e autorização com tokens JWT
+70. Salvando perfis de usuário na base de dados
+ROLE_ADMIN e ROLE_CLIENTE - no tipo enumerado Perfil, o prefixo "ROLE_" é uma exigência do Spring Security - padroes de escrita exigidas do framework</t>
+  </si>
+  <si>
+    <t>1:30
+6. Autenticação e autorização com tokens JWT
+70. Salvando perfis de usuário na base de dados
+criação de @ElementCollection(fetch=FetchType.EAGER) - é importante o FetchType.EAGER para garantir que sempre que for buscado um cliente do banco de dados, automaticamente sera buscado os PERFIS também</t>
+  </si>
+  <si>
+    <t>Salvando perfis de usuário na base de dados</t>
   </si>
 </sst>
 </file>
@@ -1524,8 +1546,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G172" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G172"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G175" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G175"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1801,10 +1823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G172"/>
+  <dimension ref="A1:G175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B169" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C173" sqref="C173"/>
+    <sheetView tabSelected="1" topLeftCell="B170" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F174" sqref="F174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4991,6 +5013,62 @@
       </c>
       <c r="G172" s="10"/>
     </row>
+    <row r="173" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B173" s="8">
+        <v>6</v>
+      </c>
+      <c r="C173" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D173" s="8">
+        <v>70</v>
+      </c>
+      <c r="E173" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="F173" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="G173" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B174" s="8">
+        <v>6</v>
+      </c>
+      <c r="C174" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D174" s="8">
+        <v>70</v>
+      </c>
+      <c r="E174" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="F174" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="G174" s="10"/>
+    </row>
+    <row r="175" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B175" s="8">
+        <v>6</v>
+      </c>
+      <c r="C175" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D175" s="8">
+        <v>70</v>
+      </c>
+      <c r="E175" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="F175" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="G175" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementando autenticacao e geracao do token JWT
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="11010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="280">
   <si>
     <t>nome aula</t>
   </si>
@@ -1284,6 +1284,98 @@
   </si>
   <si>
     <t>Salvando perfis de usuário na base de dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+6:28
+6. Autenticação e autorização com tokens JWT
+71. Implementando autenticacao e geracao do token JWT (PARTE 1)
+Criação da classe UserSS - o prefixo "SS" siginifica que será um usuário que atende o contrato/interface do Spring Security</t>
+  </si>
+  <si>
+    <t>7:52
+6. Autenticação e autorização com tokens JWT
+71. Implementando autenticacao e geracao do token JWT (PARTE 1)
+INteressante - caso queiramos implementar alguma lógica na classe UserSS, como por exemplo, algum tempo de expiração para a sessão do usuário, basta implementar nos metodos exigidos pela interface UserDetails - no caso o metodo "isAccountNonExpired"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+10:06
+6. Autenticação e autorização com tokens JWT
+71. Implementando autenticacao e geracao do token JWT (PARTE 1)
+criação da classe UserDetailServiceImpl - que implementa o contrato do Spring Security UserDetailsService - esta interface do Spring Security permite a busca pelo nome do usuário</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+12:27
+6. Autenticação e autorização com tokens JWT
+71. Implementando autenticacao e geracao do token JWT (PARTE 1)
+excessão UserNameNotFoundException do spring security por estar dentro do contexto de segurança</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+13:59
+6. Autenticação e autorização com tokens JWT
+71. Implementando autenticacao e geracao do token JWT (PARTE 1)
+criado construtor convertendo uma lista de perfis recebida por parametro para uma Collection&lt;? extends GrantedAuthority&gt; que o spring security exige</t>
+  </si>
+  <si>
+    <t>14:13
+6. Autenticação e autorização com tokens JWT
+71. Implementando autenticacao e geracao do token JWT (PARTE 1)
+em aula anterior foi observado a necessidade de usar o prefixo ROLE_ na criação do enum de perfis de usuario ... nesta aula mostra o por que deste prefixo e seu devido uso</t>
+  </si>
+  <si>
+    <t>20:10
+6. Autenticação e autorização com tokens JWT
+71. Implementando autenticacao e geracao do token JWT (PARTE 1)
+criação de chaves no arquivo application.properties para a palabra secreta que sera embaralhada no toke e o tempo de expiração (em milissegundos) da sessão/requisição</t>
+  </si>
+  <si>
+    <t>21:25
+6. Autenticação e autorização com tokens JWT
+71. Implementando autenticacao e geracao do token JWT (PARTE 1)
+criação da classe auxiliar JWT Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>23:24
+6. Autenticação e autorização com tokens JWT
+71. Implementando autenticacao e geracao do token JWT (PARTE 1)
+criação do metodo generateToken - uso da biblioteca JWT pela primeira vez - o builder contido no retorno deste metodo é quem gera o token</t>
+  </si>
+  <si>
+    <t>Implementando autenticacao e geracao do token JWT (PARTE 1)</t>
+  </si>
+  <si>
+    <t>0:11
+6. Autenticação e autorização com tokens JWT
+72. Implementando autenticacao e geracao do token JWT - PARTE 2
+criação de um filtro de autenticação - que intercepta a requisição, executa algo antes, e depois se der certo devolve a execução para a requisição continuar normalmente</t>
+  </si>
+  <si>
+    <t>1:28
+6. Autenticação e autorização com tokens JWT
+72. Implementando autenticacao e geracao do token JWT - PARTE 2
+para que este filtro seja um filtro de autenticação, e necessário estender para um filtro do Spring Security chamado UsernamePasswordAuthenticationFilter. Quando criamos uma classe que estende UsernamePasswordAuthenticationFilter, automaticamente o Spring Security saberá que este filtro terá que interceptar a requisição de login (endpoint /login)... inclusive esse endpoint de sufixo "/login" é padrao reservado do Spring Security tbm</t>
+  </si>
+  <si>
+    <t>6:44
+6. Autenticação e autorização com tokens JWT
+72. Implementando autenticacao e geracao do token JWT - PARTE 2
+fim da implementação do metodo que autentica usuario com o framework Spring Security</t>
+  </si>
+  <si>
+    <t>9:55
+6. Autenticação e autorização com tokens JWT
+72. Implementando autenticacao e geracao do token JWT - PARTE 2
+para o teste funcionar, é necessário ter inserido a atualização mencionada na aula anterior, referente ao erro 403 quando o correto é gerar um erro 401 quando o usuario insere dados invalidos de login</t>
+  </si>
+  <si>
+    <t>Implementando autenticacao e geracao do token JWT (PARTE 2)</t>
   </si>
 </sst>
 </file>
@@ -1546,8 +1638,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G175" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G175"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G188" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G188"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1823,10 +1915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G175"/>
+  <dimension ref="A1:G188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B170" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F174" sqref="F174"/>
+    <sheetView tabSelected="1" topLeftCell="A182" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E187" sqref="E187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5069,6 +5161,244 @@
       </c>
       <c r="G175" s="10"/>
     </row>
+    <row r="176" spans="2:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="B176" s="8">
+        <v>6</v>
+      </c>
+      <c r="C176" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D176" s="8">
+        <v>71</v>
+      </c>
+      <c r="E176" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F176" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="G176" s="10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="177" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B177" s="8">
+        <v>6</v>
+      </c>
+      <c r="C177" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D177" s="8">
+        <v>71</v>
+      </c>
+      <c r="E177" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F177" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="G177" s="10"/>
+    </row>
+    <row r="178" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B178" s="8">
+        <v>6</v>
+      </c>
+      <c r="C178" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D178" s="8">
+        <v>71</v>
+      </c>
+      <c r="E178" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F178" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="G178" s="10"/>
+    </row>
+    <row r="179" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B179" s="8">
+        <v>6</v>
+      </c>
+      <c r="C179" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D179" s="8">
+        <v>71</v>
+      </c>
+      <c r="E179" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F179" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G179" s="10"/>
+    </row>
+    <row r="180" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B180" s="8">
+        <v>6</v>
+      </c>
+      <c r="C180" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D180" s="8">
+        <v>71</v>
+      </c>
+      <c r="E180" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F180" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G180" s="10"/>
+    </row>
+    <row r="181" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B181" s="8">
+        <v>6</v>
+      </c>
+      <c r="C181" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D181" s="8">
+        <v>71</v>
+      </c>
+      <c r="E181" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F181" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="G181" s="10"/>
+    </row>
+    <row r="182" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B182" s="8">
+        <v>6</v>
+      </c>
+      <c r="C182" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D182" s="8">
+        <v>71</v>
+      </c>
+      <c r="E182" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F182" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="G182" s="10"/>
+    </row>
+    <row r="183" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B183" s="8">
+        <v>6</v>
+      </c>
+      <c r="C183" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D183" s="8">
+        <v>71</v>
+      </c>
+      <c r="E183" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F183" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="G183" s="10"/>
+    </row>
+    <row r="184" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B184" s="8">
+        <v>6</v>
+      </c>
+      <c r="C184" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D184" s="8">
+        <v>71</v>
+      </c>
+      <c r="E184" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F184" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="G184" s="10"/>
+    </row>
+    <row r="185" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B185" s="8">
+        <v>6</v>
+      </c>
+      <c r="C185" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D185" s="8">
+        <v>72</v>
+      </c>
+      <c r="E185" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="F185" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="G185" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="186" spans="2:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="B186" s="8">
+        <v>6</v>
+      </c>
+      <c r="C186" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D186" s="8">
+        <v>72</v>
+      </c>
+      <c r="E186" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="F186" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="G186" s="10"/>
+    </row>
+    <row r="187" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B187" s="8">
+        <v>6</v>
+      </c>
+      <c r="C187" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D187" s="8">
+        <v>72</v>
+      </c>
+      <c r="E187" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="F187" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="G187" s="10"/>
+    </row>
+    <row r="188" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B188" s="8">
+        <v>6</v>
+      </c>
+      <c r="C188" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D188" s="8">
+        <v>72</v>
+      </c>
+      <c r="E188" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="F188" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="G188" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Autorizando endpoints para perfis especificos
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="11010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="28020" windowHeight="11400"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="287">
   <si>
     <t>nome aula</t>
   </si>
@@ -1398,11 +1398,26 @@
   <si>
     <t>Implentando Autorização</t>
   </si>
+  <si>
+    <t>1:06
+6. Autenticação e autorização com tokens JWT
+74. Autorizando endpoints para perfis específicos
+Anotações @EnableGlobalMethodSecurity(prePostEnabled = true) e @PreAuthorize("hasAnyRole('ADMIN')") - tem função de dar permissoes a perfis de usuários especificos</t>
+  </si>
+  <si>
+    <t>5:30
+6. Autenticação e autorização com tokens JWT
+74. Autorizando endpoints para perfis específicos
+da permissao ao cliente  se cadastrar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Autorizando endpoints para perfis específicos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1659,8 +1674,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G191" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G191"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G193" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G193"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1928,7 +1943,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1936,10 +1951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G191"/>
+  <dimension ref="A1:G193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B185" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F191" sqref="F191"/>
+    <sheetView tabSelected="1" topLeftCell="B187" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E193" sqref="E193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5476,6 +5491,40 @@
       </c>
       <c r="G191" s="10"/>
     </row>
+    <row r="192" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B192" s="8">
+        <v>6</v>
+      </c>
+      <c r="C192" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D192" s="8">
+        <v>74</v>
+      </c>
+      <c r="E192" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F192" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="G192" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="193" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B193" s="8">
+        <v>6</v>
+      </c>
+      <c r="C193" s="9"/>
+      <c r="D193" s="8"/>
+      <c r="E193" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F193" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="G193" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Restricao de conteudo: cliente so recupera ele mesmo
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="290">
   <si>
     <t>nome aula</t>
   </si>
@@ -1412,6 +1412,21 @@
   </si>
   <si>
     <t xml:space="preserve"> Autorizando endpoints para perfis específicos</t>
+  </si>
+  <si>
+    <t>0:41
+6. Autenticação e autorização com tokens JWT
+75. Restrição de conteúdo: cliente só recupera ele mesmo
+IMPORTANTE: todo sitema que mexe com permissões possui um serviço (classe USerService) que pega o usuario logado</t>
+  </si>
+  <si>
+    <t>1:55
+6. Autenticação e autorização com tokens JWT
+75. Restrição de conteúdo: cliente só recupera ele mesmo
+criação de método que retorna um usuario logado na forma de um usuário do spring security</t>
+  </si>
+  <si>
+    <t>Restrição de conteúdo: cliente só recupera ele mesmo</t>
   </si>
 </sst>
 </file>
@@ -1674,8 +1689,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G193" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G193"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G195" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G195"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1943,7 +1958,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1951,7 +1966,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G193"/>
+  <dimension ref="A1:G195"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B187" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E193" sqref="E193"/>
@@ -5515,8 +5530,12 @@
       <c r="B193" s="8">
         <v>6</v>
       </c>
-      <c r="C193" s="9"/>
-      <c r="D193" s="8"/>
+      <c r="C193" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D193" s="8">
+        <v>74</v>
+      </c>
       <c r="E193" s="9" t="s">
         <v>286</v>
       </c>
@@ -5524,6 +5543,44 @@
         <v>285</v>
       </c>
       <c r="G193" s="10"/>
+    </row>
+    <row r="194" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B194" s="8">
+        <v>6</v>
+      </c>
+      <c r="C194" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D194" s="8">
+        <v>75</v>
+      </c>
+      <c r="E194" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="F194" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="G194" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="195" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B195" s="8">
+        <v>6</v>
+      </c>
+      <c r="C195" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D195" s="8">
+        <v>75</v>
+      </c>
+      <c r="E195" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="F195" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="G195" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Restricao de conteudo: clientes recupera seus pedidos
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="28020" windowHeight="11400"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="23730" windowHeight="7785"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="294">
   <si>
     <t>nome aula</t>
   </si>
@@ -1427,6 +1427,28 @@
   </si>
   <si>
     <t>Restrição de conteúdo: cliente só recupera ele mesmo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+0:07
+6. Autenticação e autorização com tokens JWT
+76. Restrição de conteúdo: cliente só recupera seus pedidos
+aula com ATUALIZAÇÃO</t>
+  </si>
+  <si>
+    <t>5:10
+6. Autenticação e autorização com tokens JWT
+76. Restrição de conteúdo: cliente só recupera seus pedidos
+criação de endpoint para buscar os pedidos do cliente que esta logado</t>
+  </si>
+  <si>
+    <t>5:51
+6. Autenticação e autorização com tokens JWT
+76. Restrição de conteúdo: cliente só recupera seus pedidos
+na criação do endpoint findPage não foi inserido o atributo value da anotação @RequestMapping.. pois foi reaproveitado o endpoint principal "/pedidos"</t>
+  </si>
+  <si>
+    <t>Restrição de conteúdo: cliente só recupera seus pedidos</t>
   </si>
 </sst>
 </file>
@@ -1689,8 +1711,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G195" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G195"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G198" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G198"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -1958,7 +1980,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1966,10 +1988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G195"/>
+  <dimension ref="A1:G198"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B187" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E193" sqref="E193"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C197" sqref="C197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5582,6 +5604,62 @@
       </c>
       <c r="G195" s="10"/>
     </row>
+    <row r="196" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B196" s="8">
+        <v>6</v>
+      </c>
+      <c r="C196" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D196" s="8">
+        <v>76</v>
+      </c>
+      <c r="E196" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F196" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="G196" s="10" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="197" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B197" s="8">
+        <v>6</v>
+      </c>
+      <c r="C197" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D197" s="8">
+        <v>76</v>
+      </c>
+      <c r="E197" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F197" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G197" s="10"/>
+    </row>
+    <row r="198" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B198" s="8">
+        <v>6</v>
+      </c>
+      <c r="C198" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D198" s="8">
+        <v>76</v>
+      </c>
+      <c r="E198" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F198" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="G198" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Salvando primeiro arquivo no S3
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="11010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23820" windowHeight="5835"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="319">
   <si>
     <t>nome aula</t>
   </si>
@@ -1487,6 +1487,105 @@
   </si>
   <si>
     <t>Esqueci a senha</t>
+  </si>
+  <si>
+    <t>Armazenamento de imagens usando Amazon S3</t>
+  </si>
+  <si>
+    <t>Criando um bucket no S3</t>
+  </si>
+  <si>
+    <t>0:31
+7. Armazenamento de imagens usando Amazon S3
+82. Criando um bucket no S3
+criação do bucket no s3 (AWS - Amazon) - pesquisar por all services (todos os serviços) e progurar a opção Armazenamento&gt;S3</t>
+  </si>
+  <si>
+    <t>Setup do IAM - Identity Access Management</t>
+  </si>
+  <si>
+    <t>1:02
+7. Armazenamento de imagens usando Amazon S3
+83. Setup do IAM - Identity Access Management
+configuração do IAM - Identity Access Management do AWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1:22
+7. Armazenamento de imagens usando Amazon S3
+83. Setup do IAM - Identity Access Management
+configurar MFA (Multi Factory Autenticator) - multiplica o grau de segurança do acesso ao AWS ... faz com que o acesso ao AWS nao seja apenas pela senha, mas também por um codigo gerado por um aplicativo no smartphone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1:57
+7. Armazenamento de imagens usando Amazon S3
+83. Setup do IAM - Identity Access Management
+necessário um aplicativo de authenticação .. o professor recomenda o uso do google authenticator - app que gera codigos de acesso para inserir na conta AWS ... como se fosse uma authenticação de varios fatores</t>
+  </si>
+  <si>
+    <t>3:03
+7. Armazenamento de imagens usando Amazon S3
+83. Setup do IAM - Identity Access Management
+criação de grupo de usuarios - no caso foi criado um grupo chamado "developers" ... simulando que vamos dar permissao para os desenvolvedores do projeto</t>
+  </si>
+  <si>
+    <t>3:16
+7. Armazenamento de imagens usando Amazon S3
+83. Setup do IAM - Identity Access Management
+adiciona a permissão AmazonS3FullAccess ao grupo developers</t>
+  </si>
+  <si>
+    <t>3:58
+7. Armazenamento de imagens usando Amazon S3
+83. Setup do IAM - Identity Access Management
+criação de usuário - onde damos o nome de "curso-spring-ionic-user" ... marcar a caixa "Acesso Programático", ou seja, alegando que este usuário tera acesso a algum programa que estivermos desenvolvendo</t>
+  </si>
+  <si>
+    <t>6:01
+7. Armazenamento de imagens usando Amazon S3
+83. Setup do IAM - Identity Access Management
+IMPORTANTISSIMO: após criação do usuário, o AWS mostra os dados do novo usuario, a ID da chave de acesso e a chave de acesso secreta ... é importantissimo salvar estes dados em um local seguro pois ele demonstra esses dados somente na criação, ou seja, somente uma vez.</t>
+  </si>
+  <si>
+    <t>6:15
+7. Armazenamento de imagens usando Amazon S3
+83. Setup do IAM - Identity Access Management
+o ultimo item "Aplicar uma politica de senhas do IAM" é opcional ... ele tem a função de adicionar politicas de senha aos usuários, tais como quantidade de caracteres obrigatórios na senha, letra maiúscula ou minuscula, números obrigatórios, etc...</t>
+  </si>
+  <si>
+    <t>2:24
+7. Armazenamento de imagens usando Amazon S3
+84. Salvando primeiro arquivo no S3
+alteração do arquivo application.properties - atenção ao id e access key do AWS ... inserir via variavel de ambiente por segurança... e para encontrar a região que foi inserida no S3 basta acessar o link: http://docs.aws.amazon.com/AWSEC2/latest/UserGuide/using-regions-availability-zones.html (que no caso foi utilizada a região South America (São Paulo) codigo: "sa-east-1"</t>
+  </si>
+  <si>
+    <t>3:56
+7. Armazenamento de imagens usando Amazon S3
+84. Salvando primeiro arquivo no S3
+criação da classe S3Config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+7:22
+7. Armazenamento de imagens usando Amazon S3
+84. Salvando primeiro arquivo no S3
+criação da classe S3Service</t>
+  </si>
+  <si>
+    <t>9:31
+7. Armazenamento de imagens usando Amazon S3
+84. Salvando primeiro arquivo no S3
+ao implementar o metodo uploadFile, utilizar o file do java.io e no s3client.putObject utilizar o que recebe como parametro um putObject .. pois possui 4 metodos putObject</t>
+  </si>
+  <si>
+    <t>12:37
+7. Armazenamento de imagens usando Amazon S3
+84. Salvando primeiro arquivo no S3
+injeta um teste basico direto na classe principal de projeto CursomcApplication .. apenas para testar os arquivos da aula e verificar se esta fazendo um upload de imagem</t>
+  </si>
+  <si>
+    <t>Salvando primeiro arquivo no S3</t>
   </si>
 </sst>
 </file>
@@ -1749,8 +1848,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G203" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G203"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G217" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G217"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -2026,10 +2125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G203"/>
+  <dimension ref="A1:G217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B200" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E204" sqref="E204"/>
+    <sheetView tabSelected="1" topLeftCell="B211" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E213" sqref="E213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5790,6 +5889,258 @@
       </c>
       <c r="G203" s="10"/>
     </row>
+    <row r="204" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B204" s="8">
+        <v>7</v>
+      </c>
+      <c r="C204" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D204" s="8">
+        <v>82</v>
+      </c>
+      <c r="E204" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="F204" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="G204" s="10"/>
+    </row>
+    <row r="205" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B205" s="8">
+        <v>7</v>
+      </c>
+      <c r="C205" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D205" s="8">
+        <v>83</v>
+      </c>
+      <c r="E205" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="F205" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="G205" s="10"/>
+    </row>
+    <row r="206" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="B206" s="8">
+        <v>7</v>
+      </c>
+      <c r="C206" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D206" s="8">
+        <v>83</v>
+      </c>
+      <c r="E206" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="F206" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="G206" s="10"/>
+    </row>
+    <row r="207" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="B207" s="8">
+        <v>7</v>
+      </c>
+      <c r="C207" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D207" s="8">
+        <v>83</v>
+      </c>
+      <c r="E207" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="F207" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="G207" s="10"/>
+    </row>
+    <row r="208" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B208" s="8">
+        <v>7</v>
+      </c>
+      <c r="C208" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D208" s="8">
+        <v>83</v>
+      </c>
+      <c r="E208" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="F208" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="G208" s="10"/>
+    </row>
+    <row r="209" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B209" s="8">
+        <v>7</v>
+      </c>
+      <c r="C209" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D209" s="8">
+        <v>83</v>
+      </c>
+      <c r="E209" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="F209" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="G209" s="10"/>
+    </row>
+    <row r="210" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B210" s="8">
+        <v>7</v>
+      </c>
+      <c r="C210" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D210" s="8">
+        <v>83</v>
+      </c>
+      <c r="E210" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="F210" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="G210" s="10"/>
+    </row>
+    <row r="211" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="B211" s="8">
+        <v>7</v>
+      </c>
+      <c r="C211" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D211" s="8">
+        <v>83</v>
+      </c>
+      <c r="E211" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="F211" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="G211" s="10"/>
+    </row>
+    <row r="212" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B212" s="8">
+        <v>7</v>
+      </c>
+      <c r="C212" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D212" s="8">
+        <v>83</v>
+      </c>
+      <c r="E212" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="F212" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="G212" s="10"/>
+    </row>
+    <row r="213" spans="2:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="B213" s="8">
+        <v>7</v>
+      </c>
+      <c r="C213" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D213" s="8">
+        <v>84</v>
+      </c>
+      <c r="E213" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="F213" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="G213" s="10"/>
+    </row>
+    <row r="214" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B214" s="8">
+        <v>7</v>
+      </c>
+      <c r="C214" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D214" s="8">
+        <v>84</v>
+      </c>
+      <c r="E214" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="F214" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="G214" s="10"/>
+    </row>
+    <row r="215" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B215" s="8">
+        <v>7</v>
+      </c>
+      <c r="C215" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D215" s="8">
+        <v>84</v>
+      </c>
+      <c r="E215" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="F215" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="G215" s="10"/>
+    </row>
+    <row r="216" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B216" s="8">
+        <v>7</v>
+      </c>
+      <c r="C216" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D216" s="8">
+        <v>84</v>
+      </c>
+      <c r="E216" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="F216" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="G216" s="10"/>
+    </row>
+    <row r="217" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B217" s="8">
+        <v>7</v>
+      </c>
+      <c r="C217" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D217" s="8">
+        <v>84</v>
+      </c>
+      <c r="E217" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="F217" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="G217" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Enviando imagem via endpoint
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23820" windowHeight="5835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="328">
   <si>
     <t>nome aula</t>
   </si>
@@ -1587,6 +1587,74 @@
   <si>
     <t>Salvando primeiro arquivo no S3</t>
   </si>
+  <si>
+    <t>0:30
+7. Armazenamento de imagens usando Amazon S3
+84. Salvando primeiro arquivo no S3
+ATENÇÃO: na aula o professor insere a dependencia do aws na version "LASTEST" ... isso gerou erros do tipo EXCEPTION_ACCESS_VIOLATION e fatal error. a resolução foi alterar a dependencia para alguma versão anterior, no caso, foi inserida uma versão mais utilizada</t>
+  </si>
+  <si>
+    <t>0:47
+7. Armazenamento de imagens usando Amazon S3
+85. Tornando o bucket com acesso público para leitura
+ao tornar o bucket com acesso publico, as configurações são padrao apenas muda o nome do projeto no S3 conforme descrito no video</t>
+  </si>
+  <si>
+    <t>1:20
+7. Armazenamento de imagens usando Amazon S3
+85. Tornando o bucket com acesso público para leitura
+correção 2:
+{
+"Version": "2012-10-17",
+"Statement": [
+{
+"Sid": "PublicRead",
+"Effect": "Allow",
+"Principal": {
+"AWS": "*"
+},
+"Action": [
+"s3:GetObject"
+],
+"Resource": [
+"arn:aws:s3:::NOME_DO_SEU_BUCKET/*"
+]
+}
+]
+}</t>
+  </si>
+  <si>
+    <t>1:17
+7. Armazenamento de imagens usando Amazon S3
+85. Tornando o bucket com acesso público para leitura
+correção 1 sugerida por aluno;
+Vi que algumas pessoas estão com dificuldades ao adicionar a Política de Bucket, como o S3 sofreu atualizações será preciso desativar a opção "Bloquear o acesso público a buckets e objetos concedido por meio de novas políticas públicas de ponto de acesso e bucket" e "Bloquear acesso público e entre contas a buckets e objetos por meio de qualquer política pública de bucket ou ponto de acesso" no menu Bloquear Acesso Público na mesma aba de Permissões. O código que eu consegui usar para permissão é baseado na explicação do link abaixo. Espero que possa ajudar!
+https://docs.aws.amazon.com/pt_br/AmazonS3/latest/user-guide/block-public-access-bucket.html (continua...)</t>
+  </si>
+  <si>
+    <t>Tornando o bucket com acesso público para leitura</t>
+  </si>
+  <si>
+    <t>1:08
+7. Armazenamento de imagens usando Amazon S3
+86. Enviando imagem via endpoint
+exclusão do código de teste de inserção de imagem no AWS/S3</t>
+  </si>
+  <si>
+    <t>3:47
+7. Armazenamento de imagens usando Amazon S3
+86. Enviando imagem via endpoint
+alteração do metodo uploadFile .. fazendo ele retornar uma URI ao invés de ser void</t>
+  </si>
+  <si>
+    <t>14:04
+7. Armazenamento de imagens usando Amazon S3
+86. Enviando imagem via endpoint
+alteração do nivel de acesso para o endpoint /clientes ... não permitindo o acesso total "/**" para ele e permitindo provisóriamente o caminho /picture</t>
+  </si>
+  <si>
+    <t>Enviando imagem via endpoint</t>
+  </si>
 </sst>
 </file>
 
@@ -1688,7 +1756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1715,6 +1783,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1848,8 +1919,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G217" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G217"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G224" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G224"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -2125,10 +2196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G217"/>
+  <dimension ref="A1:G224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B211" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E213" sqref="E213"/>
+    <sheetView tabSelected="1" topLeftCell="B216" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G216" sqref="G216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5979,7 +6050,7 @@
       </c>
       <c r="G208" s="10"/>
     </row>
-    <row r="209" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B209" s="8">
         <v>7</v>
       </c>
@@ -5997,7 +6068,7 @@
       </c>
       <c r="G209" s="10"/>
     </row>
-    <row r="210" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="B210" s="8">
         <v>7</v>
       </c>
@@ -6015,7 +6086,7 @@
       </c>
       <c r="G210" s="10"/>
     </row>
-    <row r="211" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="B211" s="8">
         <v>7</v>
       </c>
@@ -6033,7 +6104,7 @@
       </c>
       <c r="G211" s="10"/>
     </row>
-    <row r="212" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" s="1" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="B212" s="8">
         <v>7</v>
       </c>
@@ -6051,25 +6122,25 @@
       </c>
       <c r="G212" s="10"/>
     </row>
-    <row r="213" spans="2:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="B213" s="8">
         <v>7</v>
       </c>
-      <c r="C213" s="9" t="s">
+      <c r="C213" s="2" t="s">
         <v>301</v>
       </c>
       <c r="D213" s="8">
         <v>84</v>
       </c>
-      <c r="E213" s="9" t="s">
+      <c r="E213" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="F213" s="9" t="s">
-        <v>313</v>
+      <c r="F213" s="12" t="s">
+        <v>319</v>
       </c>
       <c r="G213" s="10"/>
     </row>
-    <row r="214" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" s="1" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="B214" s="8">
         <v>7</v>
       </c>
@@ -6083,11 +6154,11 @@
         <v>318</v>
       </c>
       <c r="F214" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="G214" s="10"/>
     </row>
-    <row r="215" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B215" s="8">
         <v>7</v>
       </c>
@@ -6101,11 +6172,11 @@
         <v>318</v>
       </c>
       <c r="F215" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G215" s="10"/>
     </row>
-    <row r="216" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B216" s="8">
         <v>7</v>
       </c>
@@ -6119,11 +6190,11 @@
         <v>318</v>
       </c>
       <c r="F216" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G216" s="10"/>
     </row>
-    <row r="217" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B217" s="8">
         <v>7</v>
       </c>
@@ -6137,9 +6208,135 @@
         <v>318</v>
       </c>
       <c r="F217" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="G217" s="10"/>
+    </row>
+    <row r="218" spans="1:7" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B218" s="8">
+        <v>7</v>
+      </c>
+      <c r="C218" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D218" s="8">
+        <v>84</v>
+      </c>
+      <c r="E218" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="F218" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="G217" s="10"/>
+      <c r="G218" s="10"/>
+    </row>
+    <row r="219" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B219" s="1">
+        <v>7</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D219" s="1">
+        <v>85</v>
+      </c>
+      <c r="E219" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F219" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G219" s="3"/>
+    </row>
+    <row r="220" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+      <c r="B220" s="1">
+        <v>7</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D220" s="1">
+        <v>85</v>
+      </c>
+      <c r="E220" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F220" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="G220" s="3"/>
+    </row>
+    <row r="221" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="B221" s="1">
+        <v>7</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D221" s="1">
+        <v>85</v>
+      </c>
+      <c r="E221" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F221" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G221" s="3"/>
+    </row>
+    <row r="222" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B222" s="1">
+        <v>7</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D222" s="1">
+        <v>86</v>
+      </c>
+      <c r="E222" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F222" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G222" s="3"/>
+    </row>
+    <row r="223" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B223" s="1">
+        <v>7</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D223" s="1">
+        <v>86</v>
+      </c>
+      <c r="E223" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F223" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="G223" s="3"/>
+    </row>
+    <row r="224" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B224" s="1">
+        <v>7</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="D224" s="1">
+        <v>86</v>
+      </c>
+      <c r="E224" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="F224" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G224" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Salvando URL da imagem em Cliente
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="336">
   <si>
     <t>nome aula</t>
   </si>
@@ -1669,6 +1669,34 @@
   </si>
   <si>
     <t>Tratando exceções adequadamente</t>
+  </si>
+  <si>
+    <t>0:17
+7. Armazenamento de imagens usando Amazon S3
+88. Salvando URL da imagem em Cliente
+abordagem provisória - salvar a URL da imagem em Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1:00
+7. Armazenamento de imagens usando Amazon S3
+88. Salvando URL da imagem em Cliente
+retirando inserção de imagem (permissão do endpoint "/clientes/picture")que foi inserida provisóriamente para testes e exigir login/autenticação para que seja inserido imagens no banco</t>
+  </si>
+  <si>
+    <t>3:58
+7. Armazenamento de imagens usando Amazon S3
+88. Salvando URL da imagem em Cliente
+no video o professor usa o "repo.FindOne(user.getId())" ao instanciar o cliente mas este metodo gera erro ... para consertar usa-se: "Cliente cli = find(user.getId());"</t>
+  </si>
+  <si>
+    <t>6:57
+7. Armazenamento de imagens usando Amazon S3
+88. Salvando URL da imagem em Cliente
+para enviar a imagem de acordo com o usuario autenticado, é necessário logar, depois pegar o token no header, acessar o endpoint, incluir a imagem junto do token para que funcione</t>
+  </si>
+  <si>
+    <t>Salvando URL da imagem em Cliente</t>
   </si>
 </sst>
 </file>
@@ -1934,8 +1962,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G226" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G226"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G230" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G230"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -2211,10 +2239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G226"/>
+  <dimension ref="A1:G230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B222" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D227" sqref="D227"/>
+    <sheetView tabSelected="1" topLeftCell="B225" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E231" sqref="E231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6391,6 +6419,80 @@
       </c>
       <c r="G226" s="10"/>
     </row>
+    <row r="227" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B227" s="8">
+        <v>7</v>
+      </c>
+      <c r="C227" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D227" s="8">
+        <v>88</v>
+      </c>
+      <c r="E227" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="F227" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="G227" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="228" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B228" s="8">
+        <v>7</v>
+      </c>
+      <c r="C228" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D228" s="8">
+        <v>88</v>
+      </c>
+      <c r="E228" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="F228" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="G228" s="10"/>
+    </row>
+    <row r="229" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B229" s="8">
+        <v>7</v>
+      </c>
+      <c r="C229" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D229" s="8">
+        <v>88</v>
+      </c>
+      <c r="E229" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="F229" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="G229" s="10"/>
+    </row>
+    <row r="230" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B230" s="8">
+        <v>7</v>
+      </c>
+      <c r="C230" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D230" s="8">
+        <v>88</v>
+      </c>
+      <c r="E230" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="F230" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="G230" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Usando pardão de nomes para imagens
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="339">
   <si>
     <t>nome aula</t>
   </si>
@@ -1698,6 +1698,21 @@
   <si>
     <t>Salvando URL da imagem em Cliente</t>
   </si>
+  <si>
+    <t>5:01
+7. Armazenamento de imagens usando Amazon S3
+89. Usando padrão de nomes para imagens
+implementa metodo que pega um arquivo do tipo MultipartFile e converte para um BufferedImage</t>
+  </si>
+  <si>
+    <t>9:43
+7. Armazenamento de imagens usando Amazon S3
+89. Usando padrão de nomes para imagens
+fim da implementação de um metodo que retorna um InputStream pois o método que faz o upload no S3 recebe um InputStream</t>
+  </si>
+  <si>
+    <t>Usando padrão de nomes para imagens</t>
+  </si>
 </sst>
 </file>
 
@@ -1799,7 +1814,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1829,6 +1844,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1962,8 +1980,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G230" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G230"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G232" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G232"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -2239,10 +2257,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G230"/>
+  <dimension ref="A1:G235"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B225" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E231" sqref="E231"/>
+      <selection activeCell="E233" sqref="E233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6493,6 +6511,47 @@
       </c>
       <c r="G230" s="10"/>
     </row>
+    <row r="231" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B231" s="8">
+        <v>7</v>
+      </c>
+      <c r="C231" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D231" s="8">
+        <v>89</v>
+      </c>
+      <c r="E231" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="F231" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="G231" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="232" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B232" s="8">
+        <v>7</v>
+      </c>
+      <c r="C232" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D232" s="8">
+        <v>89</v>
+      </c>
+      <c r="E232" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="F232" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="G232" s="10"/>
+    </row>
+    <row r="233" spans="2:7" x14ac:dyDescent="0.25"/>
+    <row r="234" spans="2:7" x14ac:dyDescent="0.25"/>
+    <row r="235" spans="2:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Bonus: ajustando tamanho da imagem
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="343">
   <si>
     <t>nome aula</t>
   </si>
@@ -1712,6 +1712,26 @@
   </si>
   <si>
     <t>Usando padrão de nomes para imagens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+2:13
+7. Armazenamento de imagens usando Amazon S3
+90. Bônus: ajustando tamanho da imagem
+bonus - ajuste no tamanho da imagem para envio para o amazon, ajustando proporções e reduzindo o tamanho em disco para ficar leve na requisição</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>2:28
+7. Armazenamento de imagens usando Amazon S3
+90. Bônus: ajustando tamanho da imagem
+inclusão de dependência que tem função de tratar/editar a imagem</t>
+  </si>
+  <si>
+    <t>Bônus: ajustando tamanho da imagem</t>
   </si>
 </sst>
 </file>
@@ -1980,8 +2000,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G232" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G232"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G234" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G234"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -2259,8 +2279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B225" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E233" sqref="E233"/>
+    <sheetView tabSelected="1" topLeftCell="B232" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F234" sqref="F234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6549,8 +6569,44 @@
       </c>
       <c r="G232" s="10"/>
     </row>
-    <row r="233" spans="2:7" x14ac:dyDescent="0.25"/>
-    <row r="234" spans="2:7" x14ac:dyDescent="0.25"/>
+    <row r="233" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B233" s="8">
+        <v>7</v>
+      </c>
+      <c r="C233" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D233" s="8">
+        <v>90</v>
+      </c>
+      <c r="E233" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="F233" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="G233" s="10" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="234" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B234" s="8">
+        <v>7</v>
+      </c>
+      <c r="C234" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="D234" s="8">
+        <v>90</v>
+      </c>
+      <c r="E234" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="F234" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="G234" s="10"/>
+    </row>
     <row r="235" spans="2:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Endpoint para buscar cliente por email
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="11010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="353">
   <si>
     <t>nome aula</t>
   </si>
@@ -1732,6 +1732,68 @@
   </si>
   <si>
     <t>Bônus: ajustando tamanho da imagem</t>
+  </si>
+  <si>
+    <t>0:47
+8. Ajustes finais no backend e bucket
+93. Expondo o header Authorization (problema de Cors)
+na classe JWTAuthenticationFilter, nossa aplicação nao consegue acessar a adição de header "res.addHeader("Authorization", "Bearer " + token);" no metodo "successfulAuthentication"</t>
+  </si>
+  <si>
+    <t>1:21
+8. Ajustes finais no backend e bucket
+93. Expondo o header Authorization (problema de Cors)
+Cors (Cross-origin resource sharing) - é um mecanismo que tem a função de informar quais recursos (ex. HTTP, headers) estarão disponiveis para requisições advindas de origens diferentes</t>
+  </si>
+  <si>
+    <t>3:44
+8. Ajustes finais no backend e bucket
+93. Expondo o header Authorization (problema de Cors)
+ATENÇÃO/IMPORTANTE -  um pequeno nivelamento sobre o CORS e sua devida importancia, conforme fluxograma no link: https://upload.wikimedia.org/wikipedia/commons/c/ca/Flowchart_showing_Simple_and_Preflight_XHR.svg
+mais infos nos links disponibilizados no material de apoio do capitulo;
+https://stackoverflow.com/questions/1256593/why-am-i-getting-an-options-request-instead-of-a-get-request
+https://stackoverflow.com/questions/47687774/how-to-access-headers-from-a-httpclient-response-angular-ionic
+https://www.html5rocks.com/en/tutorials/cors/</t>
+  </si>
+  <si>
+    <t>Ajustes finais no backend e no bucket</t>
+  </si>
+  <si>
+    <t>Expondo o header Authorization (problema de Cors)</t>
+  </si>
+  <si>
+    <t>0:09
+8. Ajustes finais no backend e bucket
+94. Configuração de Cors no bucket
+atualização nas configurações de Cors no bucket - inserção de instrução especifica aceitando todas origens HTTP e HTTPS para o bucket;
+&lt;?xml version="1.0" encoding="UTF-8"?&gt;
+&lt;CORSConfiguration xmlns="http://s3.amazonaws.com/doc/2006-03-01/"&gt;
+&lt;CORSRule&gt;
+&lt;AllowedOrigin&gt;http://*&lt;/AllowedOrigin&gt;
+&lt;AllowedOrigin&gt;https://*&lt;/AllowedOrigin&gt;
+&lt;AllowedMethod&gt;GET&lt;/AllowedMethod&gt;
+&lt;MaxAgeSeconds&gt;3000&lt;/MaxAgeSeconds&gt;
+&lt;AllowedHeader&gt;Authorization&lt;/AllowedHeader&gt;
+&lt;/CORSRule&gt;
+&lt;/CORSConfiguration&gt;</t>
+  </si>
+  <si>
+    <t>Configuração de Cors no bucket</t>
+  </si>
+  <si>
+    <t>0:21
+8. Ajustes finais no backend e bucket
+96. Endpoint para buscar cliente por email
+localmente, nossa aplicação armazenara somente o carrinho de compras e o token do usuário logado, pois o token carrega o nome de usuário e o tempo de expiração.</t>
+  </si>
+  <si>
+    <t>5:00
+8. Ajustes finais no backend e bucket
+96. Endpoint para buscar cliente por email
+quando o usuário logado tiver perfil de ADMINISTRADOR, ele consegue buscar qualquer e-mail/cliente</t>
+  </si>
+  <si>
+    <t>Endpoint para buscar cliente por email</t>
   </si>
 </sst>
 </file>
@@ -2000,8 +2062,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G234" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G234"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G240" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G240"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -2277,10 +2339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G235"/>
+  <dimension ref="A1:G240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B232" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F234" sqref="F234"/>
+    <sheetView tabSelected="1" topLeftCell="B238" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B240" sqref="B240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6589,7 +6651,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="234" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B234" s="8">
         <v>7</v>
       </c>
@@ -6605,9 +6667,120 @@
       <c r="F234" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="G234" s="10"/>
-    </row>
-    <row r="235" spans="2:7" x14ac:dyDescent="0.25"/>
+      <c r="G234" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="235" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B235" s="8">
+        <v>8</v>
+      </c>
+      <c r="C235" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D235" s="8">
+        <v>93</v>
+      </c>
+      <c r="E235" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="F235" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="G235" s="10"/>
+    </row>
+    <row r="236" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B236" s="8">
+        <v>8</v>
+      </c>
+      <c r="C236" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D236" s="8">
+        <v>93</v>
+      </c>
+      <c r="E236" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="F236" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="G236" s="10"/>
+    </row>
+    <row r="237" spans="2:7" ht="255" x14ac:dyDescent="0.25">
+      <c r="B237" s="8">
+        <v>8</v>
+      </c>
+      <c r="C237" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D237" s="8">
+        <v>93</v>
+      </c>
+      <c r="E237" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="F237" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="G237" s="10"/>
+    </row>
+    <row r="238" spans="2:7" ht="405" x14ac:dyDescent="0.25">
+      <c r="B238" s="8">
+        <v>8</v>
+      </c>
+      <c r="C238" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D238" s="8">
+        <v>94</v>
+      </c>
+      <c r="E238" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="F238" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="G238" s="10"/>
+    </row>
+    <row r="239" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B239" s="8">
+        <v>8</v>
+      </c>
+      <c r="C239" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D239" s="8">
+        <v>96</v>
+      </c>
+      <c r="E239" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="F239" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="G239" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="240" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B240" s="8">
+        <v>8</v>
+      </c>
+      <c r="C240" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D240" s="8">
+        <v>96</v>
+      </c>
+      <c r="E240" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="F240" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="G240" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Endpoint para buscar estados e cidades
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="11010"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="360">
   <si>
     <t>nome aula</t>
   </si>
@@ -1794,6 +1794,45 @@
   </si>
   <si>
     <t>Endpoint para buscar cliente por email</t>
+  </si>
+  <si>
+    <t>2:07
+8. Ajustes finais no backend e bucket
+97. Endpoints para buscar estados e cidades
+utilização de padrão de nomes do spring data</t>
+  </si>
+  <si>
+    <t>3:42
+8. Ajustes finais no backend e bucket
+97. Endpoints para buscar estados e cidades
+sempre importante lembrar de colocar a anotação @Service ... caso contrário os objetos não serão injetaveis</t>
+  </si>
+  <si>
+    <t>3:52
+8. Ajustes finais no backend e bucket
+97. Endpoints para buscar estados e cidades
+IMPORTANTE: as classes services tem a unção de repassar a chamada para a camada repository</t>
+  </si>
+  <si>
+    <t>4:08
+8. Ajustes finais no backend e bucket
+97. Endpoints para buscar estados e cidades
+criação de endpoint EstadoResource para acessar os "/estados"</t>
+  </si>
+  <si>
+    <t>9:13
+8. Ajustes finais no backend e bucket
+97. Endpoints para buscar estados e cidades
+sugestão do professor (implementado na aula e no projeto): criação do endpoint para obter cidades direto no EstadoResource invés de criar no resource de cidades</t>
+  </si>
+  <si>
+    <t>10:05
+8. Ajustes finais no backend e bucket
+97. Endpoints para buscar estados e cidades
+IMPORTANTE: endpoint dentro de chaves {} significa que ele recebe um parametro de URL. Ex. "/{estadoId}/cidades" ... este caso recebe as cidades de acordo com o parametro estadoId, ou seja, recebe as cidades de acordo com o estado</t>
+  </si>
+  <si>
+    <t>Endpoints para buscar estados e cidades</t>
   </si>
 </sst>
 </file>
@@ -2062,8 +2101,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G240" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G240"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G246" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G246"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -2339,10 +2378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G240"/>
+  <dimension ref="A1:G246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B238" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B240" sqref="B240"/>
+    <sheetView tabSelected="1" topLeftCell="A239" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F245" sqref="F245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6781,6 +6820,114 @@
       </c>
       <c r="G240" s="10"/>
     </row>
+    <row r="241" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B241" s="8">
+        <v>8</v>
+      </c>
+      <c r="C241" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D241" s="8">
+        <v>97</v>
+      </c>
+      <c r="E241" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="F241" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="G241" s="10"/>
+    </row>
+    <row r="242" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B242" s="8">
+        <v>8</v>
+      </c>
+      <c r="C242" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D242" s="8">
+        <v>97</v>
+      </c>
+      <c r="E242" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="F242" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="G242" s="10"/>
+    </row>
+    <row r="243" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B243" s="8">
+        <v>8</v>
+      </c>
+      <c r="C243" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D243" s="8">
+        <v>97</v>
+      </c>
+      <c r="E243" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="F243" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="G243" s="10"/>
+    </row>
+    <row r="244" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B244" s="8">
+        <v>8</v>
+      </c>
+      <c r="C244" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D244" s="8">
+        <v>97</v>
+      </c>
+      <c r="E244" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="F244" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="G244" s="10"/>
+    </row>
+    <row r="245" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B245" s="8">
+        <v>8</v>
+      </c>
+      <c r="C245" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D245" s="8">
+        <v>97</v>
+      </c>
+      <c r="E245" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="F245" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="G245" s="10"/>
+    </row>
+    <row r="246" spans="2:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="B246" s="8">
+        <v>8</v>
+      </c>
+      <c r="C246" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D246" s="8">
+        <v>97</v>
+      </c>
+      <c r="E246" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="F246" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="G246" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Padronizando o formato das excecoes
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="363">
   <si>
     <t>nome aula</t>
   </si>
@@ -1833,6 +1833,21 @@
   </si>
   <si>
     <t>Endpoints para buscar estados e cidades</t>
+  </si>
+  <si>
+    <t>2:12
+8. Ajustes finais no backend e bucket
+98. Padronizando formato das exceções
+padronizando os erros/exceptions de acordo com os erros do framework</t>
+  </si>
+  <si>
+    <t>5:27
+8. Ajustes finais no backend e bucket
+98. Padronizando formato das exceções
+ATENÇÃO: TROCAR CÓDIGO DE ERRO DE VALIDAÇÃO PARA 422 (UNPROCESSABLE_ENTITY) ... necessário para diferenciar quando for um erro de validação ou quando for um erro diferente</t>
+  </si>
+  <si>
+    <t>Padronizando formato das exceções</t>
   </si>
 </sst>
 </file>
@@ -2101,8 +2116,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G246" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G246"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G248" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G248"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -2378,10 +2393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G246"/>
+  <dimension ref="A1:G248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F245" sqref="F245"/>
+    <sheetView tabSelected="1" topLeftCell="A240" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E249" sqref="E249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6928,6 +6943,44 @@
       </c>
       <c r="G246" s="10"/>
     </row>
+    <row r="247" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B247" s="8">
+        <v>8</v>
+      </c>
+      <c r="C247" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D247" s="8">
+        <v>98</v>
+      </c>
+      <c r="E247" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="F247" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="G247" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="248" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B248" s="8">
+        <v>8</v>
+      </c>
+      <c r="C248" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D248" s="8">
+        <v>98</v>
+      </c>
+      <c r="E248" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="F248" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="G248" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Liberando CORS para PUT e DELETE
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="11010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28020" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="366">
   <si>
     <t>nome aula</t>
   </si>
@@ -1848,6 +1848,21 @@
   </si>
   <si>
     <t>Padronizando formato das exceções</t>
+  </si>
+  <si>
+    <t>0:25
+8. Ajustes finais no backend e bucket
+100. Liberando CORS para PUT e DELETE
+liberando CORS para PUT e DELETE (EM TESTES NAO DEU O ERRO INDUZIDO NA AULA - TALVEZ DEVIDO A VERSAO ATUALIZADA)  - como o backend necessita de autorização/autenticação ... as configurações que estavam do metodo corsConfigurationSource () na classe SecurityConfig da problema na requisição</t>
+  </si>
+  <si>
+    <t>1:01
+8. Ajustes finais no backend e bucket
+100. Liberando CORS para PUT e DELETE
+o professor inclui uma alteração neste método para corrigir problemas de cors. No teste realizado no video, causa um erro no postman chamado "Invalid CORS request". No meu teste local este erro não foi gerado, acredito ser devido a versão do framework. De qualquer forma, para aprendizado, foi implementado mesmo assim a correção sugerida</t>
+  </si>
+  <si>
+    <t>Liberando CORS para PUT e DELETE</t>
   </si>
 </sst>
 </file>
@@ -2116,8 +2131,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G248" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G248"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G250" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G250"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -2393,10 +2408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G248"/>
+  <dimension ref="A1:G250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A240" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E249" sqref="E249"/>
+    <sheetView tabSelected="1" topLeftCell="A244" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D249" sqref="D249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6981,6 +6996,44 @@
       </c>
       <c r="G248" s="10"/>
     </row>
+    <row r="249" spans="2:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="B249" s="8">
+        <v>8</v>
+      </c>
+      <c r="C249" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D249" s="8">
+        <v>100</v>
+      </c>
+      <c r="E249" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="F249" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="G249" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="250" spans="2:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="B250" s="8">
+        <v>8</v>
+      </c>
+      <c r="C250" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D250" s="8">
+        <v>100</v>
+      </c>
+      <c r="E250" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="F250" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="G250" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Expondo o header location nas respostas
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="369">
   <si>
     <t>nome aula</t>
   </si>
@@ -1863,6 +1863,21 @@
   </si>
   <si>
     <t>Liberando CORS para PUT e DELETE</t>
+  </si>
+  <si>
+    <t>0:48
+8. Ajustes finais no backend e bucket
+101. Expondo o header location nas respostas
+expondo o header "location" no cabeçalho de retorno da requisição através de filter/filtro ... em uma requisição para inserir algum dado por exemplo, ele gera um novo id ou endpoint ou novo recurso... o header location é justamente para isso, retornar a URL do novo recurso criado... ist é necessário pois o ANGULAR vai precisar enxergar este cabeçalho location</t>
+  </si>
+  <si>
+    <t>4:31
+8. Ajustes finais no backend e bucket
+101. Expondo o header location nas respostas
+anotação @Component - o professor não comentou nada sobre a anotação mas pelo que eu entendi, ela tem a função de interceptar todas requisições - neste caso foi criado a classe HeaderExposureFilter para aplicar um filtro que expoe o cabeçalho "location" ... em nenhum outro local nós chamamos algum metodo desta classe ou se quer chamamos a classe. O que me leva a crer que a simples anotação @Component faz este trabalho de interceptação</t>
+  </si>
+  <si>
+    <t>Expondo o header location nas respostas</t>
   </si>
 </sst>
 </file>
@@ -2131,8 +2146,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G250" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G250"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G252" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G252"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -2408,10 +2423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G250"/>
+  <dimension ref="A1:G252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D249" sqref="D249"/>
+    <sheetView tabSelected="1" topLeftCell="B247" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E252" sqref="E252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7034,6 +7049,44 @@
       </c>
       <c r="G250" s="10"/>
     </row>
+    <row r="251" spans="2:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="B251" s="8">
+        <v>8</v>
+      </c>
+      <c r="C251" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D251" s="8">
+        <v>101</v>
+      </c>
+      <c r="E251" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="F251" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="G251" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="252" spans="2:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="B252" s="8">
+        <v>8</v>
+      </c>
+      <c r="C252" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D252" s="8">
+        <v>101</v>
+      </c>
+      <c r="E252" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="F252" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="G252" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Aumentando o tamanho maximo permitido para upload
</commit_message>
<xml_diff>
--- a/anotacoes.xlsx
+++ b/anotacoes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="371">
   <si>
     <t>nome aula</t>
   </si>
@@ -1878,6 +1878,17 @@
   </si>
   <si>
     <t>Expondo o header location nas respostas</t>
+  </si>
+  <si>
+    <t>0:47
+8. Ajustes finais no backend e bucket
+102. Aumentando o tamanho máximo permitido para upload
+LEMBRAR DA ATUALIZAÇÃO NO INICIO DA AULA - o spring boot por padrão aceita o tamanho maximo de upload de 1mb - na aula aumentamos para 10mb
+referencias:
+https://stackoverflow.com/questions/37540028/how-to-set-the-max-size-of-upload-file</t>
+  </si>
+  <si>
+    <t>Aumentando o tamanho máximo permitido para upload</t>
   </si>
 </sst>
 </file>
@@ -2146,8 +2157,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G252" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B1:G252"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B1:G253" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B1:G253"/>
   <tableColumns count="6">
     <tableColumn id="5" name="Seção" dataDxfId="5"/>
     <tableColumn id="1" name="Nome da Seção" dataDxfId="4"/>
@@ -2423,9 +2434,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G252"/>
+  <dimension ref="A1:G253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B247" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E252" sqref="E252"/>
     </sheetView>
   </sheetViews>
@@ -7087,6 +7098,24 @@
       </c>
       <c r="G252" s="10"/>
     </row>
+    <row r="253" spans="2:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="B253" s="8">
+        <v>9</v>
+      </c>
+      <c r="C253" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="D253" s="8">
+        <v>102</v>
+      </c>
+      <c r="E253" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="F253" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="G253" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>